<commit_message>
[PWR] PWR SCH & PCB 1차 완료
</commit_message>
<xml_diff>
--- a/Plasma RF Review data.xlsx
+++ b/Plasma RF Review data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,15 @@
     <sheet name="Current Sensor" sheetId="4" r:id="rId4"/>
     <sheet name="CT" sheetId="6" r:id="rId5"/>
     <sheet name="Check list" sheetId="5" r:id="rId6"/>
+    <sheet name="Path review" sheetId="7" r:id="rId7"/>
+    <sheet name="FILTER" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="108">
   <si>
     <t>Power</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -432,6 +434,38 @@
     <t>W</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>L1[nH]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C3[pF]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fo[MHz]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VR를 원형 눈금 타입으로 변경</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Filter matching value - reference PCB의 Data와 비슷함.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -439,7 +473,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="176" formatCode="0.0"/>
-    <numFmt numFmtId="179" formatCode="0.000"/>
+    <numFmt numFmtId="177" formatCode="0.000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -981,45 +1015,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1029,9 +1033,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1040,19 +1041,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
@@ -1089,39 +1087,75 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1264,6 +1298,126 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="그림 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1333500" y="4371975"/>
+          <a:ext cx="10982325" cy="5257800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="그림 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="685800" y="666750"/>
+          <a:ext cx="10791825" cy="7915275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1561,7 +1715,7 @@
   <dimension ref="C3:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="C10" sqref="C10:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1706,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23:E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1745,7 +1899,7 @@
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="75" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="7" t="s">
@@ -1769,11 +1923,11 @@
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B7" s="22"/>
-      <c r="C7" s="17" t="s">
+      <c r="B7" s="76"/>
+      <c r="C7" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="73" t="s">
         <v>23</v>
       </c>
       <c r="E7" s="11">
@@ -1788,9 +1942,9 @@
       </c>
     </row>
     <row r="8" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="23"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="20"/>
+      <c r="B8" s="77"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="74"/>
       <c r="E8" s="13">
         <v>12</v>
       </c>
@@ -1924,7 +2078,7 @@
   <dimension ref="B4:F16"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1939,144 +2093,144 @@
       </c>
     </row>
     <row r="5" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="31" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="36"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37" t="s">
+      <c r="C6" s="26"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="F6" s="38" t="s">
+      <c r="F6" s="28" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="28">
+      <c r="E7" s="20">
         <v>48</v>
       </c>
-      <c r="F7" s="29" t="s">
+      <c r="F7" s="21" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C8" s="30"/>
-      <c r="D8" s="24" t="s">
+      <c r="C8" s="79"/>
+      <c r="D8" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="24">
+      <c r="E8" s="17">
         <v>20</v>
       </c>
-      <c r="F8" s="31" t="s">
+      <c r="F8" s="22" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C9" s="30"/>
-      <c r="D9" s="24" t="s">
+      <c r="C9" s="79"/>
+      <c r="D9" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="24">
+      <c r="E9" s="17">
         <v>4.99</v>
       </c>
-      <c r="F9" s="31" t="s">
+      <c r="F9" s="22" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="39"/>
-      <c r="D10" s="26" t="s">
+      <c r="C10" s="80"/>
+      <c r="D10" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="40">
+      <c r="E10" s="29">
         <f>E7*E9/(E8+E9)</f>
         <v>9.5846338535414155</v>
       </c>
-      <c r="F10" s="41" t="s">
+      <c r="F10" s="30" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="D11" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="28">
+      <c r="E11" s="20">
         <v>4.7</v>
       </c>
-      <c r="F11" s="29" t="s">
+      <c r="F11" s="21" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C12" s="30"/>
-      <c r="D12" s="24" t="s">
+      <c r="C12" s="79"/>
+      <c r="D12" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="24">
+      <c r="E12" s="17">
         <v>4.7</v>
       </c>
-      <c r="F12" s="31" t="s">
+      <c r="F12" s="22" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C13" s="30"/>
-      <c r="D13" s="24" t="s">
+      <c r="C13" s="79"/>
+      <c r="D13" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="25">
+      <c r="E13" s="18">
         <f>E10*E12/(E11+E12)</f>
         <v>4.7923169267707078</v>
       </c>
-      <c r="F13" s="31" t="s">
+      <c r="F13" s="22" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C14" s="30"/>
-      <c r="D14" s="24" t="s">
+      <c r="C14" s="79"/>
+      <c r="D14" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="24">
+      <c r="E14" s="17">
         <v>2.4</v>
       </c>
-      <c r="F14" s="31" t="s">
+      <c r="F14" s="22" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C15" s="30"/>
-      <c r="D15" s="24" t="s">
+      <c r="C15" s="79"/>
+      <c r="D15" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="24">
+      <c r="E15" s="17">
         <v>3.3</v>
       </c>
-      <c r="F15" s="31" t="s">
+      <c r="F15" s="22" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C16" s="32"/>
-      <c r="D16" s="33" t="s">
+      <c r="C16" s="81"/>
+      <c r="D16" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="34">
+      <c r="E16" s="24">
         <f>E13*E15/(E14+E15)</f>
         <v>2.7744992733935678</v>
       </c>
-      <c r="F16" s="35" t="s">
+      <c r="F16" s="25" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2096,8 +2250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C6:N48"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2111,7 +2265,7 @@
       </c>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C8" s="45" t="s">
+      <c r="C8" s="82" t="s">
         <v>56</v>
       </c>
       <c r="D8" s="15" t="s">
@@ -2134,7 +2288,7 @@
       </c>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C9" s="45"/>
+      <c r="C9" s="82"/>
       <c r="D9" s="15" t="s">
         <v>28</v>
       </c>
@@ -2147,12 +2301,12 @@
       <c r="G9">
         <v>0.01</v>
       </c>
-      <c r="H9" s="43" t="s">
+      <c r="H9" s="32" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="10" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C10" s="45"/>
+      <c r="C10" s="82"/>
       <c r="D10" s="15" t="s">
         <v>29</v>
       </c>
@@ -2165,49 +2319,49 @@
       <c r="G10">
         <v>0.01</v>
       </c>
-      <c r="H10" s="43" t="s">
+      <c r="H10" s="32" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="11" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C11" s="45"/>
+      <c r="C11" s="82"/>
       <c r="D11" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="E11" s="44">
+      <c r="E11" s="33">
         <f>(E8/2)*(E8/2)*E9</f>
         <v>0.390625</v>
       </c>
-      <c r="F11" s="44">
+      <c r="F11" s="33">
         <f>(F8/2)*(F8/2)*F9</f>
         <v>0.25</v>
       </c>
-      <c r="G11" s="44">
+      <c r="G11" s="33">
         <f>(G8/2)*(G8/2)*G9</f>
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="H11" s="43" t="s">
+      <c r="H11" s="32" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="12" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C12" s="45"/>
+      <c r="C12" s="82"/>
       <c r="D12" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="44">
+      <c r="E12" s="33">
         <f>E8*E9*E10/(E9+E10)</f>
         <v>6.25E-2</v>
       </c>
-      <c r="F12" s="44">
+      <c r="F12" s="33">
         <f>F8*F9*F10/(F9+F10)</f>
         <v>0.05</v>
       </c>
-      <c r="G12" s="44">
+      <c r="G12" s="33">
         <f>G8*G9*G10/(G9+G10)</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="H12" s="43" t="s">
+      <c r="H12" s="32" t="s">
         <v>33</v>
       </c>
       <c r="I12" t="s">
@@ -2215,23 +2369,23 @@
       </c>
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C13" s="45"/>
+      <c r="C13" s="82"/>
       <c r="D13" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="44">
+      <c r="E13" s="33">
         <f>E12*0.004*1000</f>
         <v>0.25</v>
       </c>
-      <c r="F13" s="44">
+      <c r="F13" s="33">
         <f>F12*0.004*1000</f>
         <v>0.2</v>
       </c>
-      <c r="G13" s="44">
+      <c r="G13" s="33">
         <f>G12*0.004*1000</f>
         <v>0.02</v>
       </c>
-      <c r="H13" s="43" t="s">
+      <c r="H13" s="32" t="s">
         <v>37</v>
       </c>
       <c r="I13" t="s">
@@ -2239,7 +2393,7 @@
       </c>
     </row>
     <row r="14" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C14" s="45"/>
+      <c r="C14" s="82"/>
       <c r="D14" s="15" t="s">
         <v>35</v>
       </c>
@@ -2252,28 +2406,28 @@
       <c r="G14">
         <v>8.25</v>
       </c>
-      <c r="H14" s="43" t="s">
+      <c r="H14" s="32" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="15" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C15" s="45"/>
+      <c r="C15" s="82"/>
       <c r="D15" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="44">
+      <c r="E15" s="33">
         <f>E14*E13</f>
         <v>2.0625</v>
       </c>
-      <c r="F15" s="44">
+      <c r="F15" s="33">
         <f>F14*F13</f>
         <v>1.6500000000000001</v>
       </c>
-      <c r="G15" s="44">
+      <c r="G15" s="33">
         <f>G14*G13</f>
         <v>0.16500000000000001</v>
       </c>
-      <c r="H15" s="43" t="s">
+      <c r="H15" s="32" t="s">
         <v>33</v>
       </c>
       <c r="I15" t="s">
@@ -2293,7 +2447,7 @@
       <c r="G16">
         <v>50</v>
       </c>
-      <c r="H16" s="43" t="s">
+      <c r="H16" s="32" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2310,7 +2464,7 @@
       <c r="G17">
         <v>10</v>
       </c>
-      <c r="H17" s="43" t="s">
+      <c r="H17" s="32" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2330,7 +2484,7 @@
         <f>(1+G16/G17)*G15</f>
         <v>0.99</v>
       </c>
-      <c r="H18" s="43" t="s">
+      <c r="H18" s="32" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2347,7 +2501,7 @@
       <c r="G19">
         <v>2.2000000000000002</v>
       </c>
-      <c r="H19" s="43" t="s">
+      <c r="H19" s="32" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2364,7 +2518,7 @@
       <c r="G20">
         <v>3.3</v>
       </c>
-      <c r="H20" s="43" t="s">
+      <c r="H20" s="32" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2384,846 +2538,846 @@
         <f>G20/(G19+G20)*G18</f>
         <v>0.59399999999999997</v>
       </c>
-      <c r="H21" s="43" t="s">
+      <c r="H21" s="32" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="22" spans="4:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="23" spans="4:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E23" s="77" t="s">
+      <c r="E23" s="86" t="s">
         <v>66</v>
       </c>
-      <c r="F23" s="78"/>
-      <c r="G23" s="78"/>
-      <c r="H23" s="79"/>
-      <c r="I23" s="80"/>
-      <c r="J23" s="81" t="s">
+      <c r="F23" s="87"/>
+      <c r="G23" s="87"/>
+      <c r="H23" s="84"/>
+      <c r="I23" s="85"/>
+      <c r="J23" s="83" t="s">
         <v>67</v>
       </c>
-      <c r="K23" s="79"/>
-      <c r="L23" s="79"/>
-      <c r="M23" s="80"/>
+      <c r="K23" s="84"/>
+      <c r="L23" s="84"/>
+      <c r="M23" s="85"/>
     </row>
     <row r="24" spans="4:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E24" s="49" t="s">
+      <c r="E24" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="F24" s="28">
+      <c r="F24" s="20">
         <v>0.01</v>
       </c>
-      <c r="G24" s="69" t="s">
+      <c r="G24" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="H24" s="46"/>
-      <c r="I24" s="47"/>
-      <c r="J24" s="54"/>
-      <c r="K24" s="46"/>
-      <c r="L24" s="46"/>
-      <c r="M24" s="47"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="35"/>
+      <c r="J24" s="42"/>
+      <c r="K24" s="34"/>
+      <c r="L24" s="34"/>
+      <c r="M24" s="35"/>
     </row>
     <row r="25" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="E25" s="70" t="s">
+      <c r="E25" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="F25" s="24">
+      <c r="F25" s="17">
         <v>0.01</v>
       </c>
-      <c r="G25" s="71" t="s">
+      <c r="G25" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="H25" s="67" t="s">
+      <c r="H25" s="55" t="s">
         <v>57</v>
       </c>
-      <c r="I25" s="55">
+      <c r="I25" s="43">
         <v>47</v>
       </c>
-      <c r="J25" s="49" t="s">
+      <c r="J25" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="K25" s="56">
+      <c r="K25" s="44">
         <v>3.6</v>
       </c>
-      <c r="L25" s="49" t="s">
+      <c r="L25" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="M25" s="56">
+      <c r="M25" s="44">
         <v>2.2000000000000002</v>
       </c>
-      <c r="N25" s="43" t="s">
+      <c r="N25" s="32" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="26" spans="4:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E26" s="72" t="s">
+      <c r="E26" s="60" t="s">
         <v>35</v>
       </c>
-      <c r="F26" s="33">
+      <c r="F26" s="23">
         <v>8.25</v>
       </c>
-      <c r="G26" s="73" t="s">
+      <c r="G26" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="H26" s="68" t="s">
+      <c r="H26" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="I26" s="53">
+      <c r="I26" s="41">
         <v>10</v>
       </c>
-      <c r="J26" s="72" t="s">
+      <c r="J26" s="60" t="s">
         <v>62</v>
       </c>
-      <c r="K26" s="57">
+      <c r="K26" s="45">
         <v>3.3</v>
       </c>
-      <c r="L26" s="72" t="s">
+      <c r="L26" s="60" t="s">
         <v>62</v>
       </c>
-      <c r="M26" s="57">
+      <c r="M26" s="45">
         <v>3.3</v>
       </c>
-      <c r="N26" s="43" t="s">
+      <c r="N26" s="32" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="27" spans="4:14" s="16" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E27" s="82" t="s">
+      <c r="E27" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="F27" s="83" t="s">
+      <c r="F27" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="G27" s="83" t="s">
+      <c r="G27" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="H27" s="83" t="s">
+      <c r="H27" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="I27" s="84" t="s">
+      <c r="I27" s="67" t="s">
         <v>65</v>
       </c>
-      <c r="J27" s="85"/>
-      <c r="K27" s="86" t="s">
+      <c r="J27" s="68"/>
+      <c r="K27" s="69" t="s">
         <v>63</v>
       </c>
-      <c r="L27" s="86" t="s">
+      <c r="L27" s="69" t="s">
         <v>63</v>
       </c>
-      <c r="M27" s="87" t="s">
+      <c r="M27" s="70" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="28" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="E28" s="74">
+      <c r="E28" s="62">
         <v>12.5</v>
       </c>
-      <c r="F28" s="75">
+      <c r="F28" s="63">
         <f>E28*F$24*F$25/(F$24+F$25)</f>
         <v>6.25E-2</v>
       </c>
-      <c r="G28" s="75">
+      <c r="G28" s="63">
         <f>F28*0.004*1000</f>
         <v>0.25</v>
       </c>
-      <c r="H28" s="75">
+      <c r="H28" s="63">
         <f>F$26*G28</f>
         <v>2.0625</v>
       </c>
-      <c r="I28" s="76">
-        <f>(1+I$25/I$26)*H28</f>
+      <c r="I28" s="64">
+        <f t="shared" ref="I28:I48" si="0">(1+I$25/I$26)*H28</f>
         <v>11.75625</v>
       </c>
-      <c r="J28" s="60"/>
-      <c r="K28" s="61">
-        <f>K$26/(K$25+K$26)*I28</f>
+      <c r="J28" s="48"/>
+      <c r="K28" s="49">
+        <f t="shared" ref="K28:K48" si="1">K$26/(K$25+K$26)*I28</f>
         <v>5.6225543478260862</v>
       </c>
-      <c r="L28" s="61">
-        <f>M$26/(M$25+M$26)*K28</f>
+      <c r="L28" s="49">
+        <f t="shared" ref="L28:L48" si="2">M$26/(M$25+M$26)*K28</f>
         <v>3.3735326086956516</v>
       </c>
-      <c r="M28" s="62">
+      <c r="M28" s="50">
         <f>L28/3.3*255</f>
         <v>260.68206521739125</v>
       </c>
     </row>
     <row r="29" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="E29" s="50">
+      <c r="E29" s="38">
         <v>12</v>
       </c>
-      <c r="F29" s="48">
+      <c r="F29" s="36">
         <f>E29*F$24*F$25/(F$24+F$25)</f>
         <v>5.9999999999999991E-2</v>
       </c>
-      <c r="G29" s="48">
-        <f t="shared" ref="G29:G48" si="0">F29*0.004*1000</f>
+      <c r="G29" s="36">
+        <f t="shared" ref="G29:G48" si="3">F29*0.004*1000</f>
         <v>0.24</v>
       </c>
-      <c r="H29" s="48">
-        <f t="shared" ref="H29:H48" si="1">F$26*G29</f>
+      <c r="H29" s="36">
+        <f t="shared" ref="H29:H48" si="4">F$26*G29</f>
         <v>1.98</v>
       </c>
-      <c r="I29" s="58">
-        <f>(1+I$25/I$26)*H29</f>
+      <c r="I29" s="46">
+        <f t="shared" si="0"/>
         <v>11.286</v>
       </c>
-      <c r="J29" s="63"/>
-      <c r="K29" s="25">
-        <f>K$26/(K$25+K$26)*I29</f>
+      <c r="J29" s="51"/>
+      <c r="K29" s="18">
+        <f t="shared" si="1"/>
         <v>5.397652173913043</v>
       </c>
-      <c r="L29" s="25">
-        <f>M$26/(M$25+M$26)*K29</f>
+      <c r="L29" s="18">
+        <f t="shared" si="2"/>
         <v>3.2385913043478256</v>
       </c>
-      <c r="M29" s="64">
-        <f t="shared" ref="M29:M48" si="2">L29/3.3*255</f>
+      <c r="M29" s="52">
+        <f t="shared" ref="M29:M48" si="5">L29/3.3*255</f>
         <v>250.25478260869562</v>
       </c>
     </row>
     <row r="30" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="E30" s="50">
+      <c r="E30" s="38">
         <v>11.5</v>
       </c>
-      <c r="F30" s="48">
+      <c r="F30" s="36">
         <f>E30*F$24*F$25/(F$24+F$25)</f>
         <v>5.7499999999999996E-2</v>
       </c>
-      <c r="G30" s="48">
+      <c r="G30" s="36">
+        <f t="shared" si="3"/>
+        <v>0.22999999999999998</v>
+      </c>
+      <c r="H30" s="36">
+        <f t="shared" si="4"/>
+        <v>1.8975</v>
+      </c>
+      <c r="I30" s="46">
         <f t="shared" si="0"/>
-        <v>0.22999999999999998</v>
-      </c>
-      <c r="H30" s="48">
+        <v>10.81575</v>
+      </c>
+      <c r="J30" s="51"/>
+      <c r="K30" s="18">
         <f t="shared" si="1"/>
-        <v>1.8975</v>
-      </c>
-      <c r="I30" s="58">
-        <f>(1+I$25/I$26)*H30</f>
-        <v>10.81575</v>
-      </c>
-      <c r="J30" s="63"/>
-      <c r="K30" s="25">
-        <f>K$26/(K$25+K$26)*I30</f>
         <v>5.1727499999999997</v>
       </c>
-      <c r="L30" s="25">
-        <f>M$26/(M$25+M$26)*K30</f>
+      <c r="L30" s="18">
+        <f t="shared" si="2"/>
         <v>3.1036499999999996</v>
       </c>
-      <c r="M30" s="64">
-        <f t="shared" si="2"/>
+      <c r="M30" s="52">
+        <f t="shared" si="5"/>
         <v>239.82749999999999</v>
       </c>
     </row>
     <row r="31" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D31" s="15"/>
-      <c r="E31" s="50">
+      <c r="E31" s="38">
         <v>11</v>
       </c>
-      <c r="F31" s="48">
-        <f t="shared" ref="F31:F48" si="3">E31*F$24*F$25/(F$24+F$25)</f>
+      <c r="F31" s="36">
+        <f t="shared" ref="F31:F48" si="6">E31*F$24*F$25/(F$24+F$25)</f>
         <v>5.5E-2</v>
       </c>
-      <c r="G31" s="48">
+      <c r="G31" s="36">
+        <f t="shared" si="3"/>
+        <v>0.22</v>
+      </c>
+      <c r="H31" s="36">
+        <f t="shared" si="4"/>
+        <v>1.8149999999999999</v>
+      </c>
+      <c r="I31" s="46">
         <f t="shared" si="0"/>
-        <v>0.22</v>
-      </c>
-      <c r="H31" s="48">
+        <v>10.345499999999999</v>
+      </c>
+      <c r="J31" s="51"/>
+      <c r="K31" s="18">
         <f t="shared" si="1"/>
-        <v>1.8149999999999999</v>
-      </c>
-      <c r="I31" s="58">
-        <f>(1+I$25/I$26)*H31</f>
-        <v>10.345499999999999</v>
-      </c>
-      <c r="J31" s="63"/>
-      <c r="K31" s="25">
-        <f>K$26/(K$25+K$26)*I31</f>
         <v>4.9478478260869556</v>
       </c>
-      <c r="L31" s="25">
-        <f>M$26/(M$25+M$26)*K31</f>
+      <c r="L31" s="18">
+        <f t="shared" si="2"/>
         <v>2.9687086956521731</v>
       </c>
-      <c r="M31" s="64">
+      <c r="M31" s="52">
+        <f t="shared" si="5"/>
+        <v>229.4002173913043</v>
+      </c>
+    </row>
+    <row r="32" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="E32" s="38">
+        <v>10.5</v>
+      </c>
+      <c r="F32" s="36">
+        <f t="shared" si="6"/>
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="G32" s="36">
+        <f t="shared" si="3"/>
+        <v>0.21000000000000002</v>
+      </c>
+      <c r="H32" s="36">
+        <f t="shared" si="4"/>
+        <v>1.7325000000000002</v>
+      </c>
+      <c r="I32" s="46">
+        <f t="shared" si="0"/>
+        <v>9.8752500000000012</v>
+      </c>
+      <c r="J32" s="51"/>
+      <c r="K32" s="18">
+        <f t="shared" si="1"/>
+        <v>4.7229456521739133</v>
+      </c>
+      <c r="L32" s="18">
         <f t="shared" si="2"/>
-        <v>229.4002173913043</v>
-      </c>
-    </row>
-    <row r="32" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="E32" s="50">
-        <v>10.5</v>
-      </c>
-      <c r="F32" s="48">
+        <v>2.833767391304348</v>
+      </c>
+      <c r="M32" s="52">
+        <f t="shared" si="5"/>
+        <v>218.97293478260872</v>
+      </c>
+    </row>
+    <row r="33" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E33" s="38">
+        <v>10</v>
+      </c>
+      <c r="F33" s="36">
+        <f t="shared" si="6"/>
+        <v>0.05</v>
+      </c>
+      <c r="G33" s="36">
         <f t="shared" si="3"/>
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="G32" s="48">
+        <v>0.2</v>
+      </c>
+      <c r="H33" s="36">
+        <f t="shared" si="4"/>
+        <v>1.6500000000000001</v>
+      </c>
+      <c r="I33" s="46">
         <f t="shared" si="0"/>
-        <v>0.21000000000000002</v>
-      </c>
-      <c r="H32" s="48">
+        <v>9.4050000000000011</v>
+      </c>
+      <c r="J33" s="51"/>
+      <c r="K33" s="18">
         <f t="shared" si="1"/>
-        <v>1.7325000000000002</v>
-      </c>
-      <c r="I32" s="58">
-        <f>(1+I$25/I$26)*H32</f>
-        <v>9.8752500000000012</v>
-      </c>
-      <c r="J32" s="63"/>
-      <c r="K32" s="25">
-        <f>K$26/(K$25+K$26)*I32</f>
-        <v>4.7229456521739133</v>
-      </c>
-      <c r="L32" s="25">
-        <f>M$26/(M$25+M$26)*K32</f>
-        <v>2.833767391304348</v>
-      </c>
-      <c r="M32" s="64">
+        <v>4.49804347826087</v>
+      </c>
+      <c r="L33" s="18">
         <f t="shared" si="2"/>
-        <v>218.97293478260872</v>
-      </c>
-    </row>
-    <row r="33" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E33" s="50">
-        <v>10</v>
-      </c>
-      <c r="F33" s="48">
+        <v>2.6988260869565219</v>
+      </c>
+      <c r="M33" s="52">
+        <f t="shared" si="5"/>
+        <v>208.54565217391306</v>
+      </c>
+    </row>
+    <row r="34" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E34" s="38">
+        <v>9.5</v>
+      </c>
+      <c r="F34" s="36">
+        <f t="shared" si="6"/>
+        <v>4.7500000000000001E-2</v>
+      </c>
+      <c r="G34" s="36">
+        <f t="shared" si="3"/>
+        <v>0.19</v>
+      </c>
+      <c r="H34" s="36">
+        <f t="shared" si="4"/>
+        <v>1.5675000000000001</v>
+      </c>
+      <c r="I34" s="46">
+        <f t="shared" si="0"/>
+        <v>8.9347500000000011</v>
+      </c>
+      <c r="J34" s="51"/>
+      <c r="K34" s="18">
+        <f t="shared" si="1"/>
+        <v>4.2731413043478259</v>
+      </c>
+      <c r="L34" s="18">
+        <f t="shared" si="2"/>
+        <v>2.5638847826086955</v>
+      </c>
+      <c r="M34" s="52">
+        <f t="shared" si="5"/>
+        <v>198.11836956521739</v>
+      </c>
+    </row>
+    <row r="35" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E35" s="38">
+        <v>9</v>
+      </c>
+      <c r="F35" s="36">
+        <f t="shared" si="6"/>
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="G35" s="36">
+        <f t="shared" si="3"/>
+        <v>0.18</v>
+      </c>
+      <c r="H35" s="36">
+        <f t="shared" si="4"/>
+        <v>1.4849999999999999</v>
+      </c>
+      <c r="I35" s="46">
+        <f t="shared" si="0"/>
+        <v>8.4644999999999992</v>
+      </c>
+      <c r="J35" s="51"/>
+      <c r="K35" s="18">
+        <f t="shared" si="1"/>
+        <v>4.0482391304347818</v>
+      </c>
+      <c r="L35" s="18">
+        <f t="shared" si="2"/>
+        <v>2.428943478260869</v>
+      </c>
+      <c r="M35" s="52">
+        <f t="shared" si="5"/>
+        <v>187.6910869565217</v>
+      </c>
+    </row>
+    <row r="36" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E36" s="38">
+        <v>8.5</v>
+      </c>
+      <c r="F36" s="36">
+        <f t="shared" si="6"/>
+        <v>4.2500000000000003E-2</v>
+      </c>
+      <c r="G36" s="36">
+        <f t="shared" si="3"/>
+        <v>0.17</v>
+      </c>
+      <c r="H36" s="36">
+        <f t="shared" si="4"/>
+        <v>1.4025000000000001</v>
+      </c>
+      <c r="I36" s="46">
+        <f t="shared" si="0"/>
+        <v>7.994250000000001</v>
+      </c>
+      <c r="J36" s="51"/>
+      <c r="K36" s="18">
+        <f t="shared" si="1"/>
+        <v>3.8233369565217394</v>
+      </c>
+      <c r="L36" s="18">
+        <f t="shared" si="2"/>
+        <v>2.2940021739130434</v>
+      </c>
+      <c r="M36" s="52">
+        <f t="shared" si="5"/>
+        <v>177.2638043478261</v>
+      </c>
+    </row>
+    <row r="37" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E37" s="38">
+        <v>8</v>
+      </c>
+      <c r="F37" s="36">
+        <f t="shared" si="6"/>
+        <v>0.04</v>
+      </c>
+      <c r="G37" s="36">
+        <f t="shared" si="3"/>
+        <v>0.16</v>
+      </c>
+      <c r="H37" s="36">
+        <f t="shared" si="4"/>
+        <v>1.32</v>
+      </c>
+      <c r="I37" s="46">
+        <f t="shared" si="0"/>
+        <v>7.5240000000000009</v>
+      </c>
+      <c r="J37" s="51"/>
+      <c r="K37" s="18">
+        <f t="shared" si="1"/>
+        <v>3.5984347826086958</v>
+      </c>
+      <c r="L37" s="18">
+        <f t="shared" si="2"/>
+        <v>2.1590608695652174</v>
+      </c>
+      <c r="M37" s="52">
+        <f t="shared" si="5"/>
+        <v>166.83652173913046</v>
+      </c>
+    </row>
+    <row r="38" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E38" s="38">
+        <v>7.5</v>
+      </c>
+      <c r="F38" s="36">
+        <f t="shared" si="6"/>
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="G38" s="36">
+        <f t="shared" si="3"/>
+        <v>0.15</v>
+      </c>
+      <c r="H38" s="36">
+        <f t="shared" si="4"/>
+        <v>1.2375</v>
+      </c>
+      <c r="I38" s="46">
+        <f t="shared" si="0"/>
+        <v>7.0537500000000009</v>
+      </c>
+      <c r="J38" s="51"/>
+      <c r="K38" s="18">
+        <f t="shared" si="1"/>
+        <v>3.3735326086956521</v>
+      </c>
+      <c r="L38" s="18">
+        <f t="shared" si="2"/>
+        <v>2.0241195652173913</v>
+      </c>
+      <c r="M38" s="52">
+        <f t="shared" si="5"/>
+        <v>156.4092391304348</v>
+      </c>
+    </row>
+    <row r="39" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E39" s="38">
+        <v>7</v>
+      </c>
+      <c r="F39" s="36">
+        <f t="shared" si="6"/>
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G39" s="36">
+        <f t="shared" si="3"/>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="H39" s="36">
+        <f t="shared" si="4"/>
+        <v>1.155</v>
+      </c>
+      <c r="I39" s="46">
+        <f t="shared" si="0"/>
+        <v>6.5835000000000008</v>
+      </c>
+      <c r="J39" s="51"/>
+      <c r="K39" s="18">
+        <f t="shared" si="1"/>
+        <v>3.1486304347826088</v>
+      </c>
+      <c r="L39" s="18">
+        <f t="shared" si="2"/>
+        <v>1.8891782608695653</v>
+      </c>
+      <c r="M39" s="52">
+        <f t="shared" si="5"/>
+        <v>145.98195652173916</v>
+      </c>
+    </row>
+    <row r="40" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E40" s="38">
+        <v>6.5</v>
+      </c>
+      <c r="F40" s="36">
+        <f t="shared" si="6"/>
+        <v>3.2500000000000001E-2</v>
+      </c>
+      <c r="G40" s="36">
+        <f t="shared" si="3"/>
+        <v>0.13</v>
+      </c>
+      <c r="H40" s="36">
+        <f t="shared" si="4"/>
+        <v>1.0725</v>
+      </c>
+      <c r="I40" s="46">
+        <f t="shared" si="0"/>
+        <v>6.1132499999999999</v>
+      </c>
+      <c r="J40" s="51"/>
+      <c r="K40" s="18">
+        <f t="shared" si="1"/>
+        <v>2.9237282608695647</v>
+      </c>
+      <c r="L40" s="18">
+        <f t="shared" si="2"/>
+        <v>1.7542369565217388</v>
+      </c>
+      <c r="M40" s="52">
+        <f t="shared" si="5"/>
+        <v>135.55467391304344</v>
+      </c>
+    </row>
+    <row r="41" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E41" s="38">
+        <v>6</v>
+      </c>
+      <c r="F41" s="36">
+        <f t="shared" si="6"/>
+        <v>2.9999999999999995E-2</v>
+      </c>
+      <c r="G41" s="36">
+        <f t="shared" si="3"/>
+        <v>0.12</v>
+      </c>
+      <c r="H41" s="36">
+        <f t="shared" si="4"/>
+        <v>0.99</v>
+      </c>
+      <c r="I41" s="46">
+        <f t="shared" si="0"/>
+        <v>5.6429999999999998</v>
+      </c>
+      <c r="J41" s="51"/>
+      <c r="K41" s="18">
+        <f t="shared" si="1"/>
+        <v>2.6988260869565215</v>
+      </c>
+      <c r="L41" s="18">
+        <f t="shared" si="2"/>
+        <v>1.6192956521739128</v>
+      </c>
+      <c r="M41" s="52">
+        <f t="shared" si="5"/>
+        <v>125.12739130434781</v>
+      </c>
+    </row>
+    <row r="42" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E42" s="38">
+        <v>5.5</v>
+      </c>
+      <c r="F42" s="36">
+        <f t="shared" si="6"/>
+        <v>2.75E-2</v>
+      </c>
+      <c r="G42" s="36">
+        <f t="shared" si="3"/>
+        <v>0.11</v>
+      </c>
+      <c r="H42" s="36">
+        <f t="shared" si="4"/>
+        <v>0.90749999999999997</v>
+      </c>
+      <c r="I42" s="46">
+        <f t="shared" si="0"/>
+        <v>5.1727499999999997</v>
+      </c>
+      <c r="J42" s="51"/>
+      <c r="K42" s="18">
+        <f t="shared" si="1"/>
+        <v>2.4739239130434778</v>
+      </c>
+      <c r="L42" s="18">
+        <f t="shared" si="2"/>
+        <v>1.4843543478260866</v>
+      </c>
+      <c r="M42" s="52">
+        <f t="shared" si="5"/>
+        <v>114.70010869565215</v>
+      </c>
+    </row>
+    <row r="43" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E43" s="38">
+        <v>5</v>
+      </c>
+      <c r="F43" s="36">
+        <f t="shared" si="6"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="G43" s="36">
+        <f t="shared" si="3"/>
+        <v>0.1</v>
+      </c>
+      <c r="H43" s="36">
+        <f t="shared" si="4"/>
+        <v>0.82500000000000007</v>
+      </c>
+      <c r="I43" s="46">
+        <f t="shared" si="0"/>
+        <v>4.7025000000000006</v>
+      </c>
+      <c r="J43" s="51"/>
+      <c r="K43" s="18">
+        <f t="shared" si="1"/>
+        <v>2.249021739130435</v>
+      </c>
+      <c r="L43" s="18">
+        <f t="shared" si="2"/>
+        <v>1.349413043478261</v>
+      </c>
+      <c r="M43" s="52">
+        <f t="shared" si="5"/>
+        <v>104.27282608695653</v>
+      </c>
+    </row>
+    <row r="44" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E44" s="38">
+        <v>4.5</v>
+      </c>
+      <c r="F44" s="36">
+        <f t="shared" si="6"/>
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="G44" s="36">
+        <f t="shared" si="3"/>
+        <v>0.09</v>
+      </c>
+      <c r="H44" s="36">
+        <f t="shared" si="4"/>
+        <v>0.74249999999999994</v>
+      </c>
+      <c r="I44" s="46">
+        <f t="shared" si="0"/>
+        <v>4.2322499999999996</v>
+      </c>
+      <c r="J44" s="51"/>
+      <c r="K44" s="18">
+        <f t="shared" si="1"/>
+        <v>2.0241195652173909</v>
+      </c>
+      <c r="L44" s="18">
+        <f t="shared" si="2"/>
+        <v>1.2144717391304345</v>
+      </c>
+      <c r="M44" s="52">
+        <f t="shared" si="5"/>
+        <v>93.845543478260851</v>
+      </c>
+    </row>
+    <row r="45" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E45" s="38">
+        <v>4</v>
+      </c>
+      <c r="F45" s="36">
+        <f t="shared" si="6"/>
+        <v>0.02</v>
+      </c>
+      <c r="G45" s="36">
+        <f t="shared" si="3"/>
+        <v>0.08</v>
+      </c>
+      <c r="H45" s="36">
+        <f t="shared" si="4"/>
+        <v>0.66</v>
+      </c>
+      <c r="I45" s="46">
+        <f t="shared" si="0"/>
+        <v>3.7620000000000005</v>
+      </c>
+      <c r="J45" s="51"/>
+      <c r="K45" s="18">
+        <f t="shared" si="1"/>
+        <v>1.7992173913043479</v>
+      </c>
+      <c r="L45" s="18">
+        <f t="shared" si="2"/>
+        <v>1.0795304347826087</v>
+      </c>
+      <c r="M45" s="52">
+        <f t="shared" si="5"/>
+        <v>83.418260869565231</v>
+      </c>
+    </row>
+    <row r="46" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E46" s="38">
+        <v>3.5</v>
+      </c>
+      <c r="F46" s="36">
+        <f t="shared" si="6"/>
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="G46" s="36">
+        <f t="shared" si="3"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H46" s="36">
+        <f t="shared" si="4"/>
+        <v>0.57750000000000001</v>
+      </c>
+      <c r="I46" s="46">
+        <f t="shared" si="0"/>
+        <v>3.2917500000000004</v>
+      </c>
+      <c r="J46" s="51"/>
+      <c r="K46" s="18">
+        <f t="shared" si="1"/>
+        <v>1.5743152173913044</v>
+      </c>
+      <c r="L46" s="18">
+        <f t="shared" si="2"/>
+        <v>0.94458913043478265</v>
+      </c>
+      <c r="M46" s="52">
+        <f t="shared" si="5"/>
+        <v>72.990978260869582</v>
+      </c>
+    </row>
+    <row r="47" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E47" s="38">
+        <v>3</v>
+      </c>
+      <c r="F47" s="36">
+        <f t="shared" si="6"/>
+        <v>1.4999999999999998E-2</v>
+      </c>
+      <c r="G47" s="36">
+        <f t="shared" si="3"/>
+        <v>0.06</v>
+      </c>
+      <c r="H47" s="36">
+        <f t="shared" si="4"/>
+        <v>0.495</v>
+      </c>
+      <c r="I47" s="46">
+        <f t="shared" si="0"/>
+        <v>2.8214999999999999</v>
+      </c>
+      <c r="J47" s="51"/>
+      <c r="K47" s="18">
+        <f t="shared" si="1"/>
+        <v>1.3494130434782607</v>
+      </c>
+      <c r="L47" s="18">
+        <f t="shared" si="2"/>
+        <v>0.8096478260869564</v>
+      </c>
+      <c r="M47" s="52">
+        <f t="shared" si="5"/>
+        <v>62.563695652173905</v>
+      </c>
+    </row>
+    <row r="48" spans="5:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E48" s="39">
+        <v>2.5</v>
+      </c>
+      <c r="F48" s="40">
+        <f t="shared" si="6"/>
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="G48" s="40">
         <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
-      <c r="G33" s="48">
+      <c r="H48" s="40">
+        <f t="shared" si="4"/>
+        <v>0.41250000000000003</v>
+      </c>
+      <c r="I48" s="47">
         <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-      <c r="H33" s="48">
+        <v>2.3512500000000003</v>
+      </c>
+      <c r="J48" s="53"/>
+      <c r="K48" s="24">
         <f t="shared" si="1"/>
-        <v>1.6500000000000001</v>
-      </c>
-      <c r="I33" s="58">
-        <f>(1+I$25/I$26)*H33</f>
-        <v>9.4050000000000011</v>
-      </c>
-      <c r="J33" s="63"/>
-      <c r="K33" s="25">
-        <f>K$26/(K$25+K$26)*I33</f>
-        <v>4.49804347826087</v>
-      </c>
-      <c r="L33" s="25">
-        <f>M$26/(M$25+M$26)*K33</f>
-        <v>2.6988260869565219</v>
-      </c>
-      <c r="M33" s="64">
+        <v>1.1245108695652175</v>
+      </c>
+      <c r="L48" s="24">
         <f t="shared" si="2"/>
-        <v>208.54565217391306</v>
-      </c>
-    </row>
-    <row r="34" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E34" s="50">
-        <v>9.5</v>
-      </c>
-      <c r="F34" s="48">
-        <f t="shared" si="3"/>
-        <v>4.7500000000000001E-2</v>
-      </c>
-      <c r="G34" s="48">
-        <f t="shared" si="0"/>
-        <v>0.19</v>
-      </c>
-      <c r="H34" s="48">
-        <f t="shared" si="1"/>
-        <v>1.5675000000000001</v>
-      </c>
-      <c r="I34" s="58">
-        <f>(1+I$25/I$26)*H34</f>
-        <v>8.9347500000000011</v>
-      </c>
-      <c r="J34" s="63"/>
-      <c r="K34" s="25">
-        <f>K$26/(K$25+K$26)*I34</f>
-        <v>4.2731413043478259</v>
-      </c>
-      <c r="L34" s="25">
-        <f>M$26/(M$25+M$26)*K34</f>
-        <v>2.5638847826086955</v>
-      </c>
-      <c r="M34" s="64">
-        <f t="shared" si="2"/>
-        <v>198.11836956521739</v>
-      </c>
-    </row>
-    <row r="35" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E35" s="50">
-        <v>9</v>
-      </c>
-      <c r="F35" s="48">
-        <f t="shared" si="3"/>
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="G35" s="48">
-        <f t="shared" si="0"/>
-        <v>0.18</v>
-      </c>
-      <c r="H35" s="48">
-        <f t="shared" si="1"/>
-        <v>1.4849999999999999</v>
-      </c>
-      <c r="I35" s="58">
-        <f>(1+I$25/I$26)*H35</f>
-        <v>8.4644999999999992</v>
-      </c>
-      <c r="J35" s="63"/>
-      <c r="K35" s="25">
-        <f>K$26/(K$25+K$26)*I35</f>
-        <v>4.0482391304347818</v>
-      </c>
-      <c r="L35" s="25">
-        <f>M$26/(M$25+M$26)*K35</f>
-        <v>2.428943478260869</v>
-      </c>
-      <c r="M35" s="64">
-        <f t="shared" si="2"/>
-        <v>187.6910869565217</v>
-      </c>
-    </row>
-    <row r="36" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E36" s="50">
-        <v>8.5</v>
-      </c>
-      <c r="F36" s="48">
-        <f t="shared" si="3"/>
-        <v>4.2500000000000003E-2</v>
-      </c>
-      <c r="G36" s="48">
-        <f t="shared" si="0"/>
-        <v>0.17</v>
-      </c>
-      <c r="H36" s="48">
-        <f t="shared" si="1"/>
-        <v>1.4025000000000001</v>
-      </c>
-      <c r="I36" s="58">
-        <f>(1+I$25/I$26)*H36</f>
-        <v>7.994250000000001</v>
-      </c>
-      <c r="J36" s="63"/>
-      <c r="K36" s="25">
-        <f>K$26/(K$25+K$26)*I36</f>
-        <v>3.8233369565217394</v>
-      </c>
-      <c r="L36" s="25">
-        <f>M$26/(M$25+M$26)*K36</f>
-        <v>2.2940021739130434</v>
-      </c>
-      <c r="M36" s="64">
-        <f t="shared" si="2"/>
-        <v>177.2638043478261</v>
-      </c>
-    </row>
-    <row r="37" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E37" s="50">
-        <v>8</v>
-      </c>
-      <c r="F37" s="48">
-        <f t="shared" si="3"/>
-        <v>0.04</v>
-      </c>
-      <c r="G37" s="48">
-        <f t="shared" si="0"/>
-        <v>0.16</v>
-      </c>
-      <c r="H37" s="48">
-        <f t="shared" si="1"/>
-        <v>1.32</v>
-      </c>
-      <c r="I37" s="58">
-        <f>(1+I$25/I$26)*H37</f>
-        <v>7.5240000000000009</v>
-      </c>
-      <c r="J37" s="63"/>
-      <c r="K37" s="25">
-        <f>K$26/(K$25+K$26)*I37</f>
-        <v>3.5984347826086958</v>
-      </c>
-      <c r="L37" s="25">
-        <f>M$26/(M$25+M$26)*K37</f>
-        <v>2.1590608695652174</v>
-      </c>
-      <c r="M37" s="64">
-        <f t="shared" si="2"/>
-        <v>166.83652173913046</v>
-      </c>
-    </row>
-    <row r="38" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E38" s="50">
-        <v>7.5</v>
-      </c>
-      <c r="F38" s="48">
-        <f t="shared" si="3"/>
-        <v>3.7499999999999999E-2</v>
-      </c>
-      <c r="G38" s="48">
-        <f t="shared" si="0"/>
-        <v>0.15</v>
-      </c>
-      <c r="H38" s="48">
-        <f t="shared" si="1"/>
-        <v>1.2375</v>
-      </c>
-      <c r="I38" s="58">
-        <f>(1+I$25/I$26)*H38</f>
-        <v>7.0537500000000009</v>
-      </c>
-      <c r="J38" s="63"/>
-      <c r="K38" s="25">
-        <f>K$26/(K$25+K$26)*I38</f>
-        <v>3.3735326086956521</v>
-      </c>
-      <c r="L38" s="25">
-        <f>M$26/(M$25+M$26)*K38</f>
-        <v>2.0241195652173913</v>
-      </c>
-      <c r="M38" s="64">
-        <f t="shared" si="2"/>
-        <v>156.4092391304348</v>
-      </c>
-    </row>
-    <row r="39" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E39" s="50">
-        <v>7</v>
-      </c>
-      <c r="F39" s="48">
-        <f t="shared" si="3"/>
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="G39" s="48">
-        <f t="shared" si="0"/>
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="H39" s="48">
-        <f t="shared" si="1"/>
-        <v>1.155</v>
-      </c>
-      <c r="I39" s="58">
-        <f>(1+I$25/I$26)*H39</f>
-        <v>6.5835000000000008</v>
-      </c>
-      <c r="J39" s="63"/>
-      <c r="K39" s="25">
-        <f>K$26/(K$25+K$26)*I39</f>
-        <v>3.1486304347826088</v>
-      </c>
-      <c r="L39" s="25">
-        <f>M$26/(M$25+M$26)*K39</f>
-        <v>1.8891782608695653</v>
-      </c>
-      <c r="M39" s="64">
-        <f t="shared" si="2"/>
-        <v>145.98195652173916</v>
-      </c>
-    </row>
-    <row r="40" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E40" s="50">
-        <v>6.5</v>
-      </c>
-      <c r="F40" s="48">
-        <f t="shared" si="3"/>
-        <v>3.2500000000000001E-2</v>
-      </c>
-      <c r="G40" s="48">
-        <f t="shared" si="0"/>
-        <v>0.13</v>
-      </c>
-      <c r="H40" s="48">
-        <f t="shared" si="1"/>
-        <v>1.0725</v>
-      </c>
-      <c r="I40" s="58">
-        <f>(1+I$25/I$26)*H40</f>
-        <v>6.1132499999999999</v>
-      </c>
-      <c r="J40" s="63"/>
-      <c r="K40" s="25">
-        <f>K$26/(K$25+K$26)*I40</f>
-        <v>2.9237282608695647</v>
-      </c>
-      <c r="L40" s="25">
-        <f>M$26/(M$25+M$26)*K40</f>
-        <v>1.7542369565217388</v>
-      </c>
-      <c r="M40" s="64">
-        <f t="shared" si="2"/>
-        <v>135.55467391304344</v>
-      </c>
-    </row>
-    <row r="41" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E41" s="50">
-        <v>6</v>
-      </c>
-      <c r="F41" s="48">
-        <f t="shared" si="3"/>
-        <v>2.9999999999999995E-2</v>
-      </c>
-      <c r="G41" s="48">
-        <f t="shared" si="0"/>
-        <v>0.12</v>
-      </c>
-      <c r="H41" s="48">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-      <c r="I41" s="58">
-        <f>(1+I$25/I$26)*H41</f>
-        <v>5.6429999999999998</v>
-      </c>
-      <c r="J41" s="63"/>
-      <c r="K41" s="25">
-        <f>K$26/(K$25+K$26)*I41</f>
-        <v>2.6988260869565215</v>
-      </c>
-      <c r="L41" s="25">
-        <f>M$26/(M$25+M$26)*K41</f>
-        <v>1.6192956521739128</v>
-      </c>
-      <c r="M41" s="64">
-        <f t="shared" si="2"/>
-        <v>125.12739130434781</v>
-      </c>
-    </row>
-    <row r="42" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E42" s="50">
-        <v>5.5</v>
-      </c>
-      <c r="F42" s="48">
-        <f t="shared" si="3"/>
-        <v>2.75E-2</v>
-      </c>
-      <c r="G42" s="48">
-        <f t="shared" si="0"/>
-        <v>0.11</v>
-      </c>
-      <c r="H42" s="48">
-        <f t="shared" si="1"/>
-        <v>0.90749999999999997</v>
-      </c>
-      <c r="I42" s="58">
-        <f>(1+I$25/I$26)*H42</f>
-        <v>5.1727499999999997</v>
-      </c>
-      <c r="J42" s="63"/>
-      <c r="K42" s="25">
-        <f>K$26/(K$25+K$26)*I42</f>
-        <v>2.4739239130434778</v>
-      </c>
-      <c r="L42" s="25">
-        <f>M$26/(M$25+M$26)*K42</f>
-        <v>1.4843543478260866</v>
-      </c>
-      <c r="M42" s="64">
-        <f t="shared" si="2"/>
-        <v>114.70010869565215</v>
-      </c>
-    </row>
-    <row r="43" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E43" s="50">
-        <v>5</v>
-      </c>
-      <c r="F43" s="48">
-        <f t="shared" si="3"/>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="G43" s="48">
-        <f t="shared" si="0"/>
-        <v>0.1</v>
-      </c>
-      <c r="H43" s="48">
-        <f t="shared" si="1"/>
-        <v>0.82500000000000007</v>
-      </c>
-      <c r="I43" s="58">
-        <f>(1+I$25/I$26)*H43</f>
-        <v>4.7025000000000006</v>
-      </c>
-      <c r="J43" s="63"/>
-      <c r="K43" s="25">
-        <f>K$26/(K$25+K$26)*I43</f>
-        <v>2.249021739130435</v>
-      </c>
-      <c r="L43" s="25">
-        <f>M$26/(M$25+M$26)*K43</f>
-        <v>1.349413043478261</v>
-      </c>
-      <c r="M43" s="64">
-        <f t="shared" si="2"/>
-        <v>104.27282608695653</v>
-      </c>
-    </row>
-    <row r="44" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E44" s="50">
-        <v>4.5</v>
-      </c>
-      <c r="F44" s="48">
-        <f t="shared" si="3"/>
-        <v>2.2499999999999999E-2</v>
-      </c>
-      <c r="G44" s="48">
-        <f t="shared" si="0"/>
-        <v>0.09</v>
-      </c>
-      <c r="H44" s="48">
-        <f t="shared" si="1"/>
-        <v>0.74249999999999994</v>
-      </c>
-      <c r="I44" s="58">
-        <f>(1+I$25/I$26)*H44</f>
-        <v>4.2322499999999996</v>
-      </c>
-      <c r="J44" s="63"/>
-      <c r="K44" s="25">
-        <f>K$26/(K$25+K$26)*I44</f>
-        <v>2.0241195652173909</v>
-      </c>
-      <c r="L44" s="25">
-        <f>M$26/(M$25+M$26)*K44</f>
-        <v>1.2144717391304345</v>
-      </c>
-      <c r="M44" s="64">
-        <f t="shared" si="2"/>
-        <v>93.845543478260851</v>
-      </c>
-    </row>
-    <row r="45" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E45" s="50">
-        <v>4</v>
-      </c>
-      <c r="F45" s="48">
-        <f t="shared" si="3"/>
-        <v>0.02</v>
-      </c>
-      <c r="G45" s="48">
-        <f t="shared" si="0"/>
-        <v>0.08</v>
-      </c>
-      <c r="H45" s="48">
-        <f t="shared" si="1"/>
-        <v>0.66</v>
-      </c>
-      <c r="I45" s="58">
-        <f>(1+I$25/I$26)*H45</f>
-        <v>3.7620000000000005</v>
-      </c>
-      <c r="J45" s="63"/>
-      <c r="K45" s="25">
-        <f>K$26/(K$25+K$26)*I45</f>
-        <v>1.7992173913043479</v>
-      </c>
-      <c r="L45" s="25">
-        <f>M$26/(M$25+M$26)*K45</f>
-        <v>1.0795304347826087</v>
-      </c>
-      <c r="M45" s="64">
-        <f t="shared" si="2"/>
-        <v>83.418260869565231</v>
-      </c>
-    </row>
-    <row r="46" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E46" s="50">
-        <v>3.5</v>
-      </c>
-      <c r="F46" s="48">
-        <f t="shared" si="3"/>
-        <v>1.7500000000000002E-2</v>
-      </c>
-      <c r="G46" s="48">
-        <f t="shared" si="0"/>
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="H46" s="48">
-        <f t="shared" si="1"/>
-        <v>0.57750000000000001</v>
-      </c>
-      <c r="I46" s="58">
-        <f>(1+I$25/I$26)*H46</f>
-        <v>3.2917500000000004</v>
-      </c>
-      <c r="J46" s="63"/>
-      <c r="K46" s="25">
-        <f>K$26/(K$25+K$26)*I46</f>
-        <v>1.5743152173913044</v>
-      </c>
-      <c r="L46" s="25">
-        <f>M$26/(M$25+M$26)*K46</f>
-        <v>0.94458913043478265</v>
-      </c>
-      <c r="M46" s="64">
-        <f t="shared" si="2"/>
-        <v>72.990978260869582</v>
-      </c>
-    </row>
-    <row r="47" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E47" s="50">
-        <v>3</v>
-      </c>
-      <c r="F47" s="48">
-        <f t="shared" si="3"/>
-        <v>1.4999999999999998E-2</v>
-      </c>
-      <c r="G47" s="48">
-        <f t="shared" si="0"/>
-        <v>0.06</v>
-      </c>
-      <c r="H47" s="48">
-        <f t="shared" si="1"/>
-        <v>0.495</v>
-      </c>
-      <c r="I47" s="58">
-        <f>(1+I$25/I$26)*H47</f>
-        <v>2.8214999999999999</v>
-      </c>
-      <c r="J47" s="63"/>
-      <c r="K47" s="25">
-        <f>K$26/(K$25+K$26)*I47</f>
-        <v>1.3494130434782607</v>
-      </c>
-      <c r="L47" s="25">
-        <f>M$26/(M$25+M$26)*K47</f>
-        <v>0.8096478260869564</v>
-      </c>
-      <c r="M47" s="64">
-        <f t="shared" si="2"/>
-        <v>62.563695652173905</v>
-      </c>
-    </row>
-    <row r="48" spans="5:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E48" s="51">
-        <v>2.5</v>
-      </c>
-      <c r="F48" s="52">
-        <f t="shared" si="3"/>
-        <v>1.2500000000000001E-2</v>
-      </c>
-      <c r="G48" s="52">
-        <f t="shared" si="0"/>
-        <v>0.05</v>
-      </c>
-      <c r="H48" s="52">
-        <f t="shared" si="1"/>
-        <v>0.41250000000000003</v>
-      </c>
-      <c r="I48" s="59">
-        <f>(1+I$25/I$26)*H48</f>
-        <v>2.3512500000000003</v>
-      </c>
-      <c r="J48" s="65"/>
-      <c r="K48" s="34">
-        <f>K$26/(K$25+K$26)*I48</f>
-        <v>1.1245108695652175</v>
-      </c>
-      <c r="L48" s="34">
-        <f>M$26/(M$25+M$26)*K48</f>
         <v>0.67470652173913048</v>
       </c>
-      <c r="M48" s="66">
-        <f t="shared" si="2"/>
+      <c r="M48" s="54">
+        <f t="shared" si="5"/>
         <v>52.136413043478264</v>
       </c>
     </row>
@@ -3244,7 +3398,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C5:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Y7" sqref="Y7"/>
     </sheetView>
   </sheetViews>
@@ -3274,7 +3428,7 @@
       <c r="E6">
         <v>820</v>
       </c>
-      <c r="F6" s="71" t="s">
+      <c r="F6" s="59" t="s">
         <v>97</v>
       </c>
     </row>
@@ -3319,10 +3473,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:D8"/>
+  <dimension ref="B5:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3375,8 +3529,356 @@
         <v>46</v>
       </c>
     </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C9" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" t="s">
+        <v>103</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C7:V29"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="U31" sqref="U31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="P7">
+        <v>680</v>
+      </c>
+      <c r="Q7">
+        <v>820</v>
+      </c>
+      <c r="R7">
+        <f t="shared" ref="R7:R17" si="0">1/(2*3.14*(P7*Q7*10^(-21))^0.5)/1000000</f>
+        <v>6.7434008092669409</v>
+      </c>
+    </row>
+    <row r="8" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E8" t="s">
+        <v>102</v>
+      </c>
+      <c r="P8">
+        <v>680</v>
+      </c>
+      <c r="Q8">
+        <v>680</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="0"/>
+        <v>7.4051087958232937</v>
+      </c>
+    </row>
+    <row r="9" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <v>470</v>
+      </c>
+      <c r="D9">
+        <v>300</v>
+      </c>
+      <c r="E9">
+        <f>1/(2*3.14*(C9*D9*10^(-21))^0.5)/1000000</f>
+        <v>13.410062437364953</v>
+      </c>
+      <c r="M9">
+        <v>820</v>
+      </c>
+      <c r="P9">
+        <v>680</v>
+      </c>
+      <c r="Q9">
+        <v>560</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="0"/>
+        <v>8.1600324610946249</v>
+      </c>
+    </row>
+    <row r="10" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="J10">
+        <v>100</v>
+      </c>
+      <c r="M10">
+        <v>680</v>
+      </c>
+      <c r="P10">
+        <v>680</v>
+      </c>
+      <c r="Q10">
+        <v>470</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="0"/>
+        <v>8.9071131829143706</v>
+      </c>
+    </row>
+    <row r="11" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="J11">
+        <v>120</v>
+      </c>
+      <c r="M11">
+        <v>560</v>
+      </c>
+      <c r="P11">
+        <v>680</v>
+      </c>
+      <c r="Q11">
+        <v>390</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="0"/>
+        <v>9.7780802306742576</v>
+      </c>
+    </row>
+    <row r="12" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="J12">
+        <v>150</v>
+      </c>
+      <c r="M12">
+        <v>470</v>
+      </c>
+      <c r="P12">
+        <v>680</v>
+      </c>
+      <c r="Q12">
+        <v>330</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="0"/>
+        <v>10.629893905942531</v>
+      </c>
+    </row>
+    <row r="13" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="J13">
+        <v>180</v>
+      </c>
+      <c r="M13">
+        <v>390</v>
+      </c>
+      <c r="P13">
+        <v>680</v>
+      </c>
+      <c r="Q13">
+        <v>300</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="0"/>
+        <v>11.148726783662498</v>
+      </c>
+    </row>
+    <row r="14" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="J14">
+        <v>220</v>
+      </c>
+      <c r="M14">
+        <v>330</v>
+      </c>
+      <c r="P14">
+        <v>680</v>
+      </c>
+      <c r="Q14">
+        <v>270</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="0"/>
+        <v>11.751789882432261</v>
+      </c>
+    </row>
+    <row r="15" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="J15">
+        <v>330</v>
+      </c>
+      <c r="M15">
+        <v>300</v>
+      </c>
+      <c r="P15">
+        <v>680</v>
+      </c>
+      <c r="Q15">
+        <v>240</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="0"/>
+        <v>12.464655475420971</v>
+      </c>
+    </row>
+    <row r="16" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="J16">
+        <v>390</v>
+      </c>
+      <c r="M16">
+        <v>270</v>
+      </c>
+      <c r="P16">
+        <v>680</v>
+      </c>
+      <c r="Q16">
+        <v>220</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="0"/>
+        <v>13.01890804473982</v>
+      </c>
+      <c r="U16">
+        <v>12</v>
+      </c>
+      <c r="V16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <v>820</v>
+      </c>
+      <c r="D17">
+        <v>150</v>
+      </c>
+      <c r="E17">
+        <f>1/(2*3.14*(C17*D17*10^(-21))^0.5)/1000000</f>
+        <v>14.357796730373126</v>
+      </c>
+      <c r="J17">
+        <v>470</v>
+      </c>
+      <c r="M17">
+        <v>240</v>
+      </c>
+      <c r="P17">
+        <v>680</v>
+      </c>
+      <c r="Q17">
+        <v>200</v>
+      </c>
+      <c r="R17">
+        <f t="shared" si="0"/>
+        <v>13.65434595083669</v>
+      </c>
+      <c r="U17">
+        <v>3</v>
+      </c>
+      <c r="V17" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="J18">
+        <v>680</v>
+      </c>
+      <c r="M18">
+        <v>220</v>
+      </c>
+      <c r="U18">
+        <f>U17/U16</f>
+        <v>0.25</v>
+      </c>
+      <c r="V18" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C19">
+        <v>51</v>
+      </c>
+      <c r="D19">
+        <v>240</v>
+      </c>
+      <c r="E19">
+        <f>1/(2*3.14*(C19*D19*10^(-21))^0.5)/1000000</f>
+        <v>45.514486502788969</v>
+      </c>
+    </row>
+    <row r="20" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C20">
+        <v>510</v>
+      </c>
+      <c r="D20">
+        <v>2700</v>
+      </c>
+      <c r="E20">
+        <f>1/(2*3.14*(C20*D20*10^(-21))^0.5)/1000000</f>
+        <v>4.2911469397794235</v>
+      </c>
+    </row>
+    <row r="23" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="U23">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="24" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="U24">
+        <v>1.27</v>
+      </c>
+    </row>
+    <row r="25" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="U25">
+        <f>U23-U24</f>
+        <v>2.0299999999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="U26">
+        <f>U25/2</f>
+        <v>1.0149999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="U28">
+        <v>1.27</v>
+      </c>
+    </row>
+    <row r="29" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="U29">
+        <f>U28/2</f>
+        <v>0.63500000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T21" sqref="T21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[RF Gen] Pre-amp matching
</commit_message>
<xml_diff>
--- a/Plasma RF Review data.xlsx
+++ b/Plasma RF Review data.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21425"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F5905B-8C1A-444C-9FEC-CC164697F03E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,15 +14,17 @@
     <sheet name="Current Sensor" sheetId="4" r:id="rId4"/>
     <sheet name="CT" sheetId="6" r:id="rId5"/>
     <sheet name="Check list" sheetId="5" r:id="rId6"/>
-    <sheet name="Path review" sheetId="7" r:id="rId7"/>
-    <sheet name="FILTER" sheetId="8" r:id="rId8"/>
+    <sheet name="Pre-Amp" sheetId="9" r:id="rId7"/>
+    <sheet name="Path review" sheetId="7" r:id="rId8"/>
+    <sheet name="Debugging" sheetId="10" r:id="rId9"/>
+    <sheet name="FILTER" sheetId="8" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="159">
   <si>
     <t>Power</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -474,16 +477,238 @@
     <t>Fc</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>VR1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vcc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V_gate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Icc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spec</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RF Freq</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MHz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Harmonic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dBc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Power</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reflect Power</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>max</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bias</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RF_in</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RF_out</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VR1[눈금]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R1[KΩ]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R23[KΩ]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L2[uH]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gain</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>R2[K</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>Ω]</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Q1의 Gain이 0.3정도밖에 안나옴 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R4가 18.2가 아니라 18.2K가 실장되어 있었음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vpp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vrms</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vrms_cal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MRF1513NT1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pcc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>VR1[K</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>Ω]</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[V/V]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C6[pF]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C7[pF]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C34[pF]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L11[nH]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L3[nH]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L12[nH]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C3[pF]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L1[nH]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RF_IN의 +Vpp가 saturation됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RF_IN의 +Vpp가 개선</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RL=50 : TX1 1차에서 50저항 처리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="176" formatCode="0.0"/>
     <numFmt numFmtId="177" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -522,8 +747,24 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -536,8 +777,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="34">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -972,12 +1225,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -1115,6 +1405,57 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="6" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1166,6 +1507,36 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="6" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1201,7 +1572,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="그림 2"/>
+        <xdr:cNvPr id="3" name="그림 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1244,7 +1621,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="그림 1"/>
+        <xdr:cNvPr id="2" name="그림 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1287,7 +1670,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="그림 1"/>
+        <xdr:cNvPr id="2" name="그림 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1317,20 +1706,81 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>398780</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>213360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="그림 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E95DC7C-B503-45DA-91C3-7F68809D288D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5153660" y="4450080"/>
+          <a:ext cx="5415280" cy="4061460"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>647700</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>542925</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>200025</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="그림 1"/>
+        <xdr:cNvPr id="2" name="그림 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1370,10 +1820,110 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>198120</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>119380</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="그림 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{657D87C9-85E8-4F4D-8FE4-B1F4E680F3E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="868680" y="12367260"/>
+          <a:ext cx="5415280" cy="4061460"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>156210</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>20955</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="그림 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF265551-9AC3-4959-B81E-44F497B4CF6C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6911340" y="12363450"/>
+          <a:ext cx="5417820" cy="4063365"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1390,7 +1940,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="그림 1"/>
+        <xdr:cNvPr id="2" name="그림 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1476,7 +2032,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1509,9 +2065,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1544,6 +2117,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1719,173 +2309,266 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:M12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B3:P16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:F12"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="2" width="5.09765625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C3" t="s">
+    <row r="3" spans="2:16" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B3" s="31" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="C4" s="94" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="95"/>
+      <c r="E4" s="20">
+        <v>13.56</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="G4" s="44"/>
+      <c r="N4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="C5" s="92" t="s">
+        <v>117</v>
+      </c>
+      <c r="D5" s="93"/>
+      <c r="E5" s="17">
+        <v>50</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="G5" s="72" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="C6" s="92" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" s="93"/>
+      <c r="E6" s="17">
+        <v>300</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="G6" s="72" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C7" s="90" t="s">
+        <v>121</v>
+      </c>
+      <c r="D7" s="91"/>
+      <c r="E7" s="23">
+        <v>30</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="G7" s="45" t="s">
+        <v>122</v>
+      </c>
+      <c r="L7" t="s">
         <v>0</v>
       </c>
-      <c r="D3">
+      <c r="M7">
         <v>1</v>
       </c>
-      <c r="E3">
+      <c r="N7">
         <v>100</v>
       </c>
-      <c r="F3">
+      <c r="O7">
         <v>300</v>
       </c>
-      <c r="G3" t="s">
+      <c r="P7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="D4">
-        <f>10*LOG(D3)</f>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="M8">
+        <f>10*LOG(M7)</f>
         <v>0</v>
       </c>
-      <c r="E4">
-        <f>10*LOG(E3)</f>
+      <c r="N8">
+        <f>10*LOG(N7)</f>
         <v>20</v>
       </c>
-      <c r="F4" s="1">
-        <f>10*LOG(F3)</f>
+      <c r="O8" s="1">
+        <f>10*LOG(O7)</f>
         <v>24.771212547196626</v>
       </c>
-      <c r="G4" t="s">
+      <c r="P8" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="D5">
-        <f>10*LOG(D3/0.001)</f>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="M9">
+        <f>10*LOG(M7/0.001)</f>
         <v>30</v>
       </c>
-      <c r="E5">
-        <f>10*LOG(E3/0.001)</f>
+      <c r="N9">
+        <f>10*LOG(N7/0.001)</f>
         <v>50</v>
       </c>
-      <c r="F5" s="1">
-        <f>10*LOG(F3/0.001)</f>
+      <c r="O9" s="1">
+        <f>10*LOG(O7/0.001)</f>
         <v>54.771212547196626</v>
       </c>
-      <c r="G5" t="s">
+      <c r="P9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C6" t="s">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="L10" t="s">
         <v>4</v>
       </c>
-      <c r="D6">
+      <c r="M10">
         <v>30</v>
       </c>
-      <c r="E6">
+      <c r="N10">
         <v>30</v>
       </c>
-      <c r="F6">
+      <c r="O10">
         <v>30</v>
       </c>
-      <c r="G6" t="s">
+      <c r="P10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="D7">
-        <f>D5-D6</f>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="M11">
+        <f>M9-M10</f>
         <v>0</v>
       </c>
-      <c r="E7">
-        <f>E5-E6</f>
+      <c r="N11">
+        <f>N9-N10</f>
         <v>20</v>
       </c>
-      <c r="F7" s="1">
-        <f>F5-F6</f>
+      <c r="O11" s="1">
+        <f>O9-O10</f>
         <v>24.771212547196626</v>
       </c>
-      <c r="G7" t="s">
+      <c r="P11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="L14" t="s">
         <v>6</v>
       </c>
-      <c r="E10" t="s">
+      <c r="N14" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C11">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="L15">
         <v>12.56</v>
       </c>
-      <c r="D11" t="s">
+      <c r="M15" t="s">
         <v>69</v>
       </c>
-      <c r="E11" s="1">
-        <f>300/C11</f>
+      <c r="N15" s="1">
+        <f>300/L15</f>
         <v>23.885350318471335</v>
       </c>
-      <c r="F11" t="s">
+      <c r="O15" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C12">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="L16">
         <v>13.56</v>
       </c>
-      <c r="D12" t="s">
+      <c r="M16" t="s">
         <v>69</v>
       </c>
-      <c r="E12" s="1">
-        <f>300/C12</f>
+      <c r="N16" s="1">
+        <f>300/L16</f>
         <v>22.123893805309734</v>
       </c>
-      <c r="F12" t="s">
+      <c r="O16" t="s">
         <v>71</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C4:D4"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="M4" r:id="rId1"/>
+    <hyperlink ref="N4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId2"/>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T21" sqref="T21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B4:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="2" width="9" style="3"/>
-    <col min="3" max="3" width="12.375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.25" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.3984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.19921875" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:11" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="K4" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:11" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B5" s="4"/>
       <c r="C5" s="5" t="s">
         <v>24</v>
@@ -1906,8 +2589,8 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="75" t="s">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B6" s="100" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="7" t="s">
@@ -1930,12 +2613,12 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B7" s="76"/>
-      <c r="C7" s="71" t="s">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B7" s="101"/>
+      <c r="C7" s="96" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="73" t="s">
+      <c r="D7" s="98" t="s">
         <v>23</v>
       </c>
       <c r="E7" s="11">
@@ -1949,10 +2632,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="77"/>
-      <c r="C8" s="72"/>
-      <c r="D8" s="74"/>
+    <row r="8" spans="2:11" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B8" s="102"/>
+      <c r="C8" s="97"/>
+      <c r="D8" s="99"/>
       <c r="E8" s="13">
         <v>12</v>
       </c>
@@ -1964,8 +2647,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:11" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="13" spans="2:11" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C13" s="5" t="s">
         <v>24</v>
       </c>
@@ -1991,7 +2674,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.4">
       <c r="C14" s="3" t="s">
         <v>72</v>
       </c>
@@ -2020,7 +2703,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.4">
       <c r="C15" s="3" t="s">
         <v>83</v>
       </c>
@@ -2049,7 +2732,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.4">
       <c r="C16" s="3" t="s">
         <v>89</v>
       </c>
@@ -2082,30 +2765,30 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B4:F16"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="4" max="4" width="12.875" customWidth="1"/>
+    <col min="4" max="4" width="12.8984375" customWidth="1"/>
     <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C5" s="31" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C6" s="26"/>
       <c r="D6" s="27"/>
       <c r="E6" s="27" t="s">
@@ -2115,8 +2798,8 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C7" s="78" t="s">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="C7" s="103" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="20" t="s">
@@ -2129,8 +2812,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C8" s="79"/>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="C8" s="104"/>
       <c r="D8" s="17" t="s">
         <v>9</v>
       </c>
@@ -2141,8 +2824,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C9" s="79"/>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="C9" s="104"/>
       <c r="D9" s="17" t="s">
         <v>10</v>
       </c>
@@ -2153,8 +2836,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="80"/>
+    <row r="10" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C10" s="105"/>
       <c r="D10" s="19" t="s">
         <v>11</v>
       </c>
@@ -2166,8 +2849,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C11" s="78" t="s">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="C11" s="103" t="s">
         <v>16</v>
       </c>
       <c r="D11" s="20" t="s">
@@ -2180,8 +2863,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C12" s="79"/>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="C12" s="104"/>
       <c r="D12" s="17" t="s">
         <v>10</v>
       </c>
@@ -2192,8 +2875,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C13" s="79"/>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="C13" s="104"/>
       <c r="D13" s="17" t="s">
         <v>13</v>
       </c>
@@ -2205,8 +2888,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C14" s="79"/>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="C14" s="104"/>
       <c r="D14" s="17" t="s">
         <v>14</v>
       </c>
@@ -2217,8 +2900,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C15" s="79"/>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="C15" s="104"/>
       <c r="D15" s="17" t="s">
         <v>15</v>
       </c>
@@ -2229,8 +2912,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C16" s="81"/>
+    <row r="16" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C16" s="106"/>
       <c r="D16" s="23" t="s">
         <v>11</v>
       </c>
@@ -2255,25 +2938,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="C6:N48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="3" max="3" width="12.75" customWidth="1"/>
+    <col min="3" max="3" width="12.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C8" s="82" t="s">
+    <row r="8" spans="3:9" x14ac:dyDescent="0.4">
+      <c r="C8" s="107" t="s">
         <v>56</v>
       </c>
       <c r="D8" s="15" t="s">
@@ -2295,8 +2978,8 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C9" s="82"/>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.4">
+      <c r="C9" s="107"/>
       <c r="D9" s="15" t="s">
         <v>28</v>
       </c>
@@ -2313,8 +2996,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C10" s="82"/>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.4">
+      <c r="C10" s="107"/>
       <c r="D10" s="15" t="s">
         <v>29</v>
       </c>
@@ -2331,8 +3014,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C11" s="82"/>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.4">
+      <c r="C11" s="107"/>
       <c r="D11" s="15" t="s">
         <v>64</v>
       </c>
@@ -2352,8 +3035,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C12" s="82"/>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.4">
+      <c r="C12" s="107"/>
       <c r="D12" s="15" t="s">
         <v>30</v>
       </c>
@@ -2376,8 +3059,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C13" s="82"/>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.4">
+      <c r="C13" s="107"/>
       <c r="D13" s="15" t="s">
         <v>34</v>
       </c>
@@ -2400,8 +3083,8 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C14" s="82"/>
+    <row r="14" spans="3:9" x14ac:dyDescent="0.4">
+      <c r="C14" s="107"/>
       <c r="D14" s="15" t="s">
         <v>35</v>
       </c>
@@ -2418,8 +3101,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C15" s="82"/>
+    <row r="15" spans="3:9" x14ac:dyDescent="0.4">
+      <c r="C15" s="107"/>
       <c r="D15" s="15" t="s">
         <v>38</v>
       </c>
@@ -2442,7 +3125,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:9" x14ac:dyDescent="0.4">
       <c r="D16" s="15" t="s">
         <v>57</v>
       </c>
@@ -2459,7 +3142,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:14" x14ac:dyDescent="0.4">
       <c r="D17" s="15" t="s">
         <v>58</v>
       </c>
@@ -2476,7 +3159,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:14" x14ac:dyDescent="0.4">
       <c r="D18" s="15" t="s">
         <v>59</v>
       </c>
@@ -2496,7 +3179,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:14" x14ac:dyDescent="0.4">
       <c r="D19" s="15" t="s">
         <v>61</v>
       </c>
@@ -2513,7 +3196,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:14" x14ac:dyDescent="0.4">
       <c r="D20" s="15" t="s">
         <v>62</v>
       </c>
@@ -2530,7 +3213,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:14" x14ac:dyDescent="0.4">
       <c r="D21" s="15" t="s">
         <v>63</v>
       </c>
@@ -2550,23 +3233,23 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="4:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="23" spans="4:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E23" s="86" t="s">
+    <row r="22" spans="4:14" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="23" spans="4:14" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="E23" s="111" t="s">
         <v>66</v>
       </c>
-      <c r="F23" s="87"/>
-      <c r="G23" s="87"/>
-      <c r="H23" s="84"/>
-      <c r="I23" s="85"/>
-      <c r="J23" s="83" t="s">
+      <c r="F23" s="112"/>
+      <c r="G23" s="112"/>
+      <c r="H23" s="109"/>
+      <c r="I23" s="110"/>
+      <c r="J23" s="108" t="s">
         <v>67</v>
       </c>
-      <c r="K23" s="84"/>
-      <c r="L23" s="84"/>
-      <c r="M23" s="85"/>
-    </row>
-    <row r="24" spans="4:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K23" s="109"/>
+      <c r="L23" s="109"/>
+      <c r="M23" s="110"/>
+    </row>
+    <row r="24" spans="4:14" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E24" s="37" t="s">
         <v>28</v>
       </c>
@@ -2583,7 +3266,7 @@
       <c r="L24" s="34"/>
       <c r="M24" s="35"/>
     </row>
-    <row r="25" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:14" x14ac:dyDescent="0.4">
       <c r="E25" s="58" t="s">
         <v>29</v>
       </c>
@@ -2615,7 +3298,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="4:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="4:14" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E26" s="60" t="s">
         <v>35</v>
       </c>
@@ -2647,7 +3330,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="4:14" s="16" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="4:14" s="16" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E27" s="65" t="s">
         <v>27</v>
       </c>
@@ -2674,7 +3357,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="4:14" x14ac:dyDescent="0.4">
       <c r="E28" s="62">
         <v>12.5</v>
       </c>
@@ -2708,7 +3391,7 @@
         <v>260.68206521739125</v>
       </c>
     </row>
-    <row r="29" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:14" x14ac:dyDescent="0.4">
       <c r="E29" s="38">
         <v>12</v>
       </c>
@@ -2742,7 +3425,7 @@
         <v>250.25478260869562</v>
       </c>
     </row>
-    <row r="30" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:14" x14ac:dyDescent="0.4">
       <c r="E30" s="38">
         <v>11.5</v>
       </c>
@@ -2776,7 +3459,7 @@
         <v>239.82749999999999</v>
       </c>
     </row>
-    <row r="31" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="4:14" x14ac:dyDescent="0.4">
       <c r="D31" s="15"/>
       <c r="E31" s="38">
         <v>11</v>
@@ -2811,7 +3494,7 @@
         <v>229.4002173913043</v>
       </c>
     </row>
-    <row r="32" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="4:14" x14ac:dyDescent="0.4">
       <c r="E32" s="38">
         <v>10.5</v>
       </c>
@@ -2845,7 +3528,7 @@
         <v>218.97293478260872</v>
       </c>
     </row>
-    <row r="33" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="5:13" x14ac:dyDescent="0.4">
       <c r="E33" s="38">
         <v>10</v>
       </c>
@@ -2879,7 +3562,7 @@
         <v>208.54565217391306</v>
       </c>
     </row>
-    <row r="34" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="5:13" x14ac:dyDescent="0.4">
       <c r="E34" s="38">
         <v>9.5</v>
       </c>
@@ -2913,7 +3596,7 @@
         <v>198.11836956521739</v>
       </c>
     </row>
-    <row r="35" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="5:13" x14ac:dyDescent="0.4">
       <c r="E35" s="38">
         <v>9</v>
       </c>
@@ -2947,7 +3630,7 @@
         <v>187.6910869565217</v>
       </c>
     </row>
-    <row r="36" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="5:13" x14ac:dyDescent="0.4">
       <c r="E36" s="38">
         <v>8.5</v>
       </c>
@@ -2981,7 +3664,7 @@
         <v>177.2638043478261</v>
       </c>
     </row>
-    <row r="37" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="5:13" x14ac:dyDescent="0.4">
       <c r="E37" s="38">
         <v>8</v>
       </c>
@@ -3015,7 +3698,7 @@
         <v>166.83652173913046</v>
       </c>
     </row>
-    <row r="38" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="5:13" x14ac:dyDescent="0.4">
       <c r="E38" s="38">
         <v>7.5</v>
       </c>
@@ -3049,7 +3732,7 @@
         <v>156.4092391304348</v>
       </c>
     </row>
-    <row r="39" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="5:13" x14ac:dyDescent="0.4">
       <c r="E39" s="38">
         <v>7</v>
       </c>
@@ -3083,7 +3766,7 @@
         <v>145.98195652173916</v>
       </c>
     </row>
-    <row r="40" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="5:13" x14ac:dyDescent="0.4">
       <c r="E40" s="38">
         <v>6.5</v>
       </c>
@@ -3117,7 +3800,7 @@
         <v>135.55467391304344</v>
       </c>
     </row>
-    <row r="41" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="5:13" x14ac:dyDescent="0.4">
       <c r="E41" s="38">
         <v>6</v>
       </c>
@@ -3151,7 +3834,7 @@
         <v>125.12739130434781</v>
       </c>
     </row>
-    <row r="42" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="5:13" x14ac:dyDescent="0.4">
       <c r="E42" s="38">
         <v>5.5</v>
       </c>
@@ -3185,7 +3868,7 @@
         <v>114.70010869565215</v>
       </c>
     </row>
-    <row r="43" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="5:13" x14ac:dyDescent="0.4">
       <c r="E43" s="38">
         <v>5</v>
       </c>
@@ -3219,7 +3902,7 @@
         <v>104.27282608695653</v>
       </c>
     </row>
-    <row r="44" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="5:13" x14ac:dyDescent="0.4">
       <c r="E44" s="38">
         <v>4.5</v>
       </c>
@@ -3253,7 +3936,7 @@
         <v>93.845543478260851</v>
       </c>
     </row>
-    <row r="45" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="5:13" x14ac:dyDescent="0.4">
       <c r="E45" s="38">
         <v>4</v>
       </c>
@@ -3287,7 +3970,7 @@
         <v>83.418260869565231</v>
       </c>
     </row>
-    <row r="46" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="5:13" x14ac:dyDescent="0.4">
       <c r="E46" s="38">
         <v>3.5</v>
       </c>
@@ -3321,7 +4004,7 @@
         <v>72.990978260869582</v>
       </c>
     </row>
-    <row r="47" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="5:13" x14ac:dyDescent="0.4">
       <c r="E47" s="38">
         <v>3</v>
       </c>
@@ -3355,7 +4038,7 @@
         <v>62.563695652173905</v>
       </c>
     </row>
-    <row r="48" spans="5:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="5:13" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E48" s="39">
         <v>2.5</v>
       </c>
@@ -3403,16 +4086,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="C5:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Y7" sqref="Y7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:6" x14ac:dyDescent="0.4">
       <c r="C5" t="s">
         <v>92</v>
       </c>
@@ -3426,7 +4109,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:6" x14ac:dyDescent="0.4">
       <c r="C6" t="s">
         <v>94</v>
       </c>
@@ -3440,7 +4123,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:6" x14ac:dyDescent="0.4">
       <c r="C7" t="s">
         <v>95</v>
       </c>
@@ -3456,7 +4139,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:6" x14ac:dyDescent="0.4">
       <c r="C8" t="s">
         <v>96</v>
       </c>
@@ -3480,20 +4163,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B5:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="3" width="9" style="15"/>
-    <col min="4" max="4" width="81.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="81.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" s="16" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B5" s="16" t="s">
         <v>40</v>
       </c>
@@ -3504,7 +4187,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B6" s="15">
         <v>1</v>
       </c>
@@ -3515,7 +4198,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B7" s="15">
         <v>2</v>
       </c>
@@ -3526,7 +4209,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B8" s="15">
         <v>3</v>
       </c>
@@ -3537,7 +4220,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.4">
       <c r="C9" s="15" t="s">
         <v>43</v>
       </c>
@@ -3552,335 +4235,1332 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:V29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39AC99BC-2C16-460C-8540-F2312C53F795}">
+  <dimension ref="B3:S19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="11" max="16" width="8.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:19" x14ac:dyDescent="0.4">
       <c r="C3" t="s">
+        <v>123</v>
+      </c>
+      <c r="I3" s="31" t="s">
+        <v>143</v>
+      </c>
+      <c r="J3" s="31"/>
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.4">
+      <c r="D4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E4">
+        <v>12</v>
+      </c>
+      <c r="G4">
+        <v>12</v>
+      </c>
+      <c r="K4" t="s">
+        <v>142</v>
+      </c>
+      <c r="L4">
+        <v>3</v>
+      </c>
+      <c r="M4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.4">
+      <c r="D5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E5">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="K5" t="s">
+        <v>132</v>
+      </c>
+      <c r="L5">
+        <v>15</v>
+      </c>
+      <c r="M5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.4">
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="K6" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6">
+        <v>12.5</v>
+      </c>
+      <c r="M6" t="s">
+        <v>7</v>
+      </c>
+      <c r="N6">
+        <f>L6*L6/50</f>
+        <v>3.125</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.4">
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.4">
+      <c r="D8" t="s">
+        <v>112</v>
+      </c>
+      <c r="E8" s="71">
+        <f>E4*E7/(SUM(E5:E7))</f>
+        <v>2.7906976744186047</v>
+      </c>
+      <c r="F8">
+        <v>2.7570000000000001</v>
+      </c>
+      <c r="G8" s="71">
+        <f>G4*G7/(SUM(G5:G7))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="D9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F9">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.4">
+      <c r="B10" s="113" t="s">
+        <v>158</v>
+      </c>
+      <c r="C10" s="114"/>
+      <c r="D10" s="114"/>
+      <c r="E10" s="114"/>
+      <c r="F10" s="114"/>
+      <c r="G10" s="114"/>
+      <c r="H10" s="115"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="95" t="s">
+        <v>124</v>
+      </c>
+      <c r="L10" s="95"/>
+      <c r="M10" s="95"/>
+      <c r="N10" s="95" t="s">
+        <v>125</v>
+      </c>
+      <c r="O10" s="95"/>
+      <c r="P10" s="95"/>
+      <c r="Q10" s="95" t="s">
+        <v>132</v>
+      </c>
+      <c r="R10" s="95"/>
+      <c r="S10" s="44"/>
+    </row>
+    <row r="11" spans="2:19" s="16" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B11" s="60" t="s">
+        <v>127</v>
+      </c>
+      <c r="C11" s="78" t="s">
+        <v>145</v>
+      </c>
+      <c r="D11" s="78" t="s">
+        <v>133</v>
+      </c>
+      <c r="E11" s="78" t="s">
+        <v>128</v>
+      </c>
+      <c r="F11" s="78" t="s">
+        <v>126</v>
+      </c>
+      <c r="G11" s="78" t="s">
+        <v>129</v>
+      </c>
+      <c r="H11" s="78" t="s">
+        <v>131</v>
+      </c>
+      <c r="I11" s="78" t="s">
+        <v>113</v>
+      </c>
+      <c r="J11" s="78" t="s">
+        <v>144</v>
+      </c>
+      <c r="K11" s="78" t="s">
+        <v>137</v>
+      </c>
+      <c r="L11" s="78" t="s">
+        <v>138</v>
+      </c>
+      <c r="M11" s="79" t="s">
+        <v>139</v>
+      </c>
+      <c r="N11" s="78" t="s">
+        <v>137</v>
+      </c>
+      <c r="O11" s="78" t="s">
+        <v>138</v>
+      </c>
+      <c r="P11" s="79" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q11" s="78" t="s">
+        <v>146</v>
+      </c>
+      <c r="R11" s="78" t="s">
+        <v>2</v>
+      </c>
+      <c r="S11" s="80" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.4">
+      <c r="B12" s="48">
+        <v>4</v>
+      </c>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20">
+        <v>1</v>
+      </c>
+      <c r="E12" s="20">
+        <v>1</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="G12" s="20">
+        <v>1</v>
+      </c>
+      <c r="H12" s="20">
+        <v>0.8</v>
+      </c>
+      <c r="I12" s="20">
+        <v>0.42</v>
+      </c>
+      <c r="J12" s="20">
+        <f>12*I12</f>
+        <v>5.04</v>
+      </c>
+      <c r="K12" s="81">
+        <v>0.72</v>
+      </c>
+      <c r="L12" s="81"/>
+      <c r="M12" s="74">
+        <f t="shared" ref="M12:M19" si="0">K12/2*0.707</f>
+        <v>0.25451999999999997</v>
+      </c>
+      <c r="N12" s="82">
+        <v>25</v>
+      </c>
+      <c r="O12" s="81"/>
+      <c r="P12" s="74">
+        <f t="shared" ref="P12:P19" si="1">N12/2*0.707</f>
+        <v>8.8375000000000004</v>
+      </c>
+      <c r="Q12" s="82">
+        <f>N12/K12</f>
+        <v>34.722222222222221</v>
+      </c>
+      <c r="R12" s="82">
+        <f>20*LOG(Q12)</f>
+        <v>30.812150244815385</v>
+      </c>
+      <c r="S12" s="44"/>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.4">
+      <c r="B13" s="51"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17">
+        <v>100</v>
+      </c>
+      <c r="I13" s="17">
+        <v>0.46</v>
+      </c>
+      <c r="J13" s="17">
+        <f t="shared" ref="J13:J19" si="2">12*I13</f>
+        <v>5.5200000000000005</v>
+      </c>
+      <c r="K13" s="36">
+        <v>0.52800000000000002</v>
+      </c>
+      <c r="L13" s="36">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="M13" s="75">
+        <f t="shared" si="0"/>
+        <v>0.18664800000000001</v>
+      </c>
+      <c r="N13" s="76">
+        <v>22.4</v>
+      </c>
+      <c r="O13" s="36">
+        <v>7.76</v>
+      </c>
+      <c r="P13" s="75">
+        <f t="shared" si="1"/>
+        <v>7.9183999999999992</v>
+      </c>
+      <c r="Q13" s="76">
+        <f t="shared" ref="Q13:Q15" si="3">N13/K13</f>
+        <v>42.424242424242422</v>
+      </c>
+      <c r="R13" s="76">
+        <f t="shared" ref="R13:R19" si="4">20*LOG(Q13)</f>
+        <v>32.552281916007011</v>
+      </c>
+      <c r="S13" s="83">
+        <f>O13*O13/50</f>
+        <v>1.2043519999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.4">
+      <c r="B14" s="51"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17">
+        <v>0.64</v>
+      </c>
+      <c r="I14" s="17">
+        <v>0.49</v>
+      </c>
+      <c r="J14" s="17">
+        <f t="shared" si="2"/>
+        <v>5.88</v>
+      </c>
+      <c r="K14" s="36">
+        <v>0.84799999999999998</v>
+      </c>
+      <c r="L14" s="36">
+        <v>0.27700000000000002</v>
+      </c>
+      <c r="M14" s="75">
+        <f t="shared" si="0"/>
+        <v>0.29976799999999998</v>
+      </c>
+      <c r="N14" s="36">
+        <v>25.2</v>
+      </c>
+      <c r="O14" s="36">
+        <v>8.92</v>
+      </c>
+      <c r="P14" s="75">
+        <f t="shared" si="1"/>
+        <v>8.908199999999999</v>
+      </c>
+      <c r="Q14" s="76">
+        <f t="shared" si="3"/>
+        <v>29.716981132075471</v>
+      </c>
+      <c r="R14" s="76">
+        <f t="shared" si="4"/>
+        <v>29.460093770496606</v>
+      </c>
+      <c r="S14" s="83">
+        <f t="shared" ref="S14:S19" si="5">O14*O14/50</f>
+        <v>1.5913280000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.4">
+      <c r="B15" s="51"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17">
+        <v>0.4</v>
+      </c>
+      <c r="J15" s="17">
+        <f t="shared" si="2"/>
+        <v>4.8000000000000007</v>
+      </c>
+      <c r="K15" s="36">
+        <v>0.84</v>
+      </c>
+      <c r="L15" s="36">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="M15" s="75">
+        <f t="shared" si="0"/>
+        <v>0.29693999999999998</v>
+      </c>
+      <c r="N15" s="36">
+        <v>21.4</v>
+      </c>
+      <c r="O15" s="36">
+        <v>7.54</v>
+      </c>
+      <c r="P15" s="75">
+        <f t="shared" si="1"/>
+        <v>7.5648999999999988</v>
+      </c>
+      <c r="Q15" s="76">
+        <f t="shared" si="3"/>
+        <v>25.476190476190474</v>
+      </c>
+      <c r="R15" s="76">
+        <f t="shared" si="4"/>
+        <v>28.122689745746182</v>
+      </c>
+      <c r="S15" s="83">
+        <f t="shared" si="5"/>
+        <v>1.137032</v>
+      </c>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.4">
+      <c r="B16" s="51"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17">
+        <v>0.35</v>
+      </c>
+      <c r="J16" s="17">
+        <f t="shared" si="2"/>
+        <v>4.1999999999999993</v>
+      </c>
+      <c r="K16" s="36">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="L16" s="36">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="M16" s="36">
+        <f t="shared" si="0"/>
+        <v>0.10180799999999998</v>
+      </c>
+      <c r="N16" s="36">
+        <v>6.6</v>
+      </c>
+      <c r="O16" s="36">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="P16" s="75">
+        <f t="shared" si="1"/>
+        <v>2.3331</v>
+      </c>
+      <c r="Q16" s="76">
+        <f t="shared" ref="Q16:Q19" si="6">N16/K16</f>
+        <v>22.916666666666668</v>
+      </c>
+      <c r="R16" s="76">
+        <f t="shared" si="4"/>
+        <v>27.203028955652755</v>
+      </c>
+      <c r="S16" s="83">
+        <f t="shared" si="5"/>
+        <v>9.5048000000000007E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.4">
+      <c r="B17" s="51"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17">
+        <v>0.33</v>
+      </c>
+      <c r="J17" s="17">
+        <f t="shared" si="2"/>
+        <v>3.96</v>
+      </c>
+      <c r="K17" s="36">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="L17" s="36">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="M17" s="36">
+        <f t="shared" si="0"/>
+        <v>9.6152000000000001E-2</v>
+      </c>
+      <c r="N17" s="36">
+        <v>6.6</v>
+      </c>
+      <c r="O17" s="36">
+        <v>2.25</v>
+      </c>
+      <c r="P17" s="36">
+        <f t="shared" si="1"/>
+        <v>2.3331</v>
+      </c>
+      <c r="Q17" s="76">
+        <f t="shared" si="6"/>
+        <v>24.264705882352938</v>
+      </c>
+      <c r="R17" s="76">
+        <f t="shared" si="4"/>
+        <v>27.699500630153398</v>
+      </c>
+      <c r="S17" s="83">
+        <f t="shared" si="5"/>
+        <v>0.10125000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.4">
+      <c r="B18" s="51"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17">
+        <v>0.23</v>
+      </c>
+      <c r="J18" s="17">
+        <f t="shared" si="2"/>
+        <v>2.7600000000000002</v>
+      </c>
+      <c r="K18" s="36">
+        <v>0.36799999999999999</v>
+      </c>
+      <c r="L18" s="36">
+        <v>0.124</v>
+      </c>
+      <c r="M18" s="36">
+        <f t="shared" si="0"/>
+        <v>0.13008799999999998</v>
+      </c>
+      <c r="N18" s="36">
+        <v>5</v>
+      </c>
+      <c r="O18" s="36">
+        <v>1.7</v>
+      </c>
+      <c r="P18" s="36">
+        <f t="shared" si="1"/>
+        <v>1.7674999999999998</v>
+      </c>
+      <c r="Q18" s="77">
+        <f t="shared" si="6"/>
+        <v>13.586956521739131</v>
+      </c>
+      <c r="R18" s="76">
+        <f t="shared" si="4"/>
+        <v>22.66244371325002</v>
+      </c>
+      <c r="S18" s="83">
+        <f t="shared" si="5"/>
+        <v>5.779999999999999E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:19" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B19" s="84">
+        <v>5</v>
+      </c>
+      <c r="C19" s="85">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="D19" s="85">
+        <v>1</v>
+      </c>
+      <c r="E19" s="85">
+        <v>1</v>
+      </c>
+      <c r="F19" s="85" t="s">
+        <v>130</v>
+      </c>
+      <c r="G19" s="85">
+        <v>1</v>
+      </c>
+      <c r="H19" s="85">
+        <v>0.64</v>
+      </c>
+      <c r="I19" s="85">
+        <v>0.3</v>
+      </c>
+      <c r="J19" s="85">
+        <f t="shared" si="2"/>
+        <v>3.5999999999999996</v>
+      </c>
+      <c r="K19" s="86">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="L19" s="86">
+        <v>0.27</v>
+      </c>
+      <c r="M19" s="86">
+        <f t="shared" si="0"/>
+        <v>0.28845599999999999</v>
+      </c>
+      <c r="N19" s="86">
+        <v>17.2</v>
+      </c>
+      <c r="O19" s="86">
+        <v>6.07</v>
+      </c>
+      <c r="P19" s="87">
+        <f t="shared" si="1"/>
+        <v>6.0801999999999996</v>
+      </c>
+      <c r="Q19" s="88">
+        <f t="shared" si="6"/>
+        <v>21.078431372549019</v>
+      </c>
+      <c r="R19" s="88">
+        <f t="shared" si="4"/>
+        <v>26.476765763073757</v>
+      </c>
+      <c r="S19" s="89">
+        <f t="shared" si="5"/>
+        <v>0.73689800000000005</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="B10:H10"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A3:W56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="4:23" x14ac:dyDescent="0.4">
+      <c r="D3" t="s">
         <v>109</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C4">
+    <row r="4" spans="4:23" x14ac:dyDescent="0.4">
+      <c r="D4">
         <v>13.56</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>10000</v>
       </c>
-      <c r="E4">
-        <f>1/(2*3.14*C4*D4*10^(-6))</f>
+      <c r="F4">
+        <f>1/(2*3.14*D4*E4*10^(-6))</f>
         <v>1.1743043421077355</v>
       </c>
     </row>
-    <row r="7" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="P7">
+    <row r="7" spans="4:23" x14ac:dyDescent="0.4">
+      <c r="Q7">
         <v>680</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>820</v>
       </c>
-      <c r="R7">
-        <f t="shared" ref="R7:R17" si="0">1/(2*3.14*(P7*Q7*10^(-21))^0.5)/1000000</f>
+      <c r="S7">
+        <f t="shared" ref="S7:S17" si="0">1/(2*3.14*(Q7*R7*10^(-21))^0.5)/1000000</f>
         <v>6.7434008092669409</v>
       </c>
     </row>
-    <row r="8" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C8" t="s">
+    <row r="8" spans="4:23" x14ac:dyDescent="0.4">
+      <c r="D8" t="s">
         <v>100</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>101</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>102</v>
-      </c>
-      <c r="P8">
-        <v>680</v>
       </c>
       <c r="Q8">
         <v>680</v>
       </c>
       <c r="R8">
+        <v>680</v>
+      </c>
+      <c r="S8">
         <f t="shared" si="0"/>
         <v>7.4051087958232937</v>
       </c>
     </row>
-    <row r="9" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C9">
+    <row r="9" spans="4:23" x14ac:dyDescent="0.4">
+      <c r="D9">
         <v>470</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>300</v>
       </c>
-      <c r="E9">
-        <f>1/(2*3.14*(C9*D9*10^(-21))^0.5)/1000000</f>
+      <c r="F9">
+        <f>1/(2*3.14*(D9*E9*10^(-21))^0.5)/1000000</f>
         <v>13.410062437364953</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>820</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <v>680</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>560</v>
       </c>
-      <c r="R9">
+      <c r="S9">
         <f t="shared" si="0"/>
         <v>8.1600324610946249</v>
       </c>
     </row>
-    <row r="10" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="J10">
+    <row r="10" spans="4:23" x14ac:dyDescent="0.4">
+      <c r="D10">
+        <v>220</v>
+      </c>
+      <c r="E10">
+        <v>300</v>
+      </c>
+      <c r="F10">
+        <f>1/(2*3.14*(D10*E10*10^(-21))^0.5)/1000000</f>
+        <v>19.600555888428783</v>
+      </c>
+      <c r="K10">
         <v>100</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>680</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <v>680</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>470</v>
       </c>
-      <c r="R10">
+      <c r="S10">
         <f t="shared" si="0"/>
         <v>8.9071131829143706</v>
       </c>
     </row>
-    <row r="11" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="J11">
+    <row r="11" spans="4:23" x14ac:dyDescent="0.4">
+      <c r="K11">
         <v>120</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>560</v>
       </c>
-      <c r="P11">
+      <c r="Q11">
         <v>680</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
         <v>390</v>
       </c>
-      <c r="R11">
+      <c r="S11">
         <f t="shared" si="0"/>
         <v>9.7780802306742576</v>
       </c>
     </row>
-    <row r="12" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="J12">
+    <row r="12" spans="4:23" x14ac:dyDescent="0.4">
+      <c r="K12">
         <v>150</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>470</v>
       </c>
-      <c r="P12">
+      <c r="Q12">
         <v>680</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <v>330</v>
       </c>
-      <c r="R12">
+      <c r="S12">
         <f t="shared" si="0"/>
         <v>10.629893905942531</v>
       </c>
     </row>
-    <row r="13" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="J13">
+    <row r="13" spans="4:23" x14ac:dyDescent="0.4">
+      <c r="K13">
         <v>180</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>390</v>
       </c>
-      <c r="P13">
+      <c r="Q13">
         <v>680</v>
       </c>
-      <c r="Q13">
+      <c r="R13">
         <v>300</v>
       </c>
-      <c r="R13">
+      <c r="S13">
         <f t="shared" si="0"/>
         <v>11.148726783662498</v>
       </c>
     </row>
-    <row r="14" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="J14">
+    <row r="14" spans="4:23" x14ac:dyDescent="0.4">
+      <c r="K14">
         <v>220</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <v>330</v>
       </c>
-      <c r="P14">
+      <c r="Q14">
         <v>680</v>
       </c>
-      <c r="Q14">
+      <c r="R14">
         <v>270</v>
       </c>
-      <c r="R14">
+      <c r="S14">
         <f t="shared" si="0"/>
         <v>11.751789882432261</v>
       </c>
     </row>
-    <row r="15" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="J15">
+    <row r="15" spans="4:23" x14ac:dyDescent="0.4">
+      <c r="K15">
         <v>330</v>
       </c>
-      <c r="M15">
+      <c r="N15">
         <v>300</v>
       </c>
-      <c r="P15">
+      <c r="Q15">
         <v>680</v>
       </c>
-      <c r="Q15">
+      <c r="R15">
         <v>240</v>
       </c>
-      <c r="R15">
+      <c r="S15">
         <f t="shared" si="0"/>
         <v>12.464655475420971</v>
       </c>
     </row>
-    <row r="16" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="J16">
+    <row r="16" spans="4:23" x14ac:dyDescent="0.4">
+      <c r="K16">
         <v>390</v>
       </c>
-      <c r="M16">
+      <c r="N16">
         <v>270</v>
       </c>
-      <c r="P16">
+      <c r="Q16">
         <v>680</v>
       </c>
-      <c r="Q16">
+      <c r="R16">
         <v>220</v>
       </c>
-      <c r="R16">
+      <c r="S16">
         <f t="shared" si="0"/>
         <v>13.01890804473982</v>
       </c>
-      <c r="U16">
+      <c r="V16">
         <v>12</v>
       </c>
-      <c r="V16" t="s">
+      <c r="W16" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C17">
+    <row r="17" spans="4:23" x14ac:dyDescent="0.4">
+      <c r="D17">
         <v>820</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>150</v>
       </c>
-      <c r="E17">
-        <f>1/(2*3.14*(C17*D17*10^(-21))^0.5)/1000000</f>
+      <c r="F17">
+        <f>1/(2*3.14*(D17*E17*10^(-21))^0.5)/1000000</f>
         <v>14.357796730373126</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>470</v>
       </c>
-      <c r="M17">
+      <c r="N17">
         <v>240</v>
       </c>
-      <c r="P17">
+      <c r="Q17">
         <v>680</v>
       </c>
-      <c r="Q17">
+      <c r="R17">
         <v>200</v>
       </c>
-      <c r="R17">
+      <c r="S17">
         <f t="shared" si="0"/>
         <v>13.65434595083669</v>
       </c>
-      <c r="U17">
+      <c r="V17">
         <v>3</v>
       </c>
-      <c r="V17" t="s">
+      <c r="W17" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="J18">
+    <row r="18" spans="4:23" x14ac:dyDescent="0.4">
+      <c r="K18">
         <v>680</v>
       </c>
-      <c r="M18">
+      <c r="N18">
         <v>220</v>
       </c>
-      <c r="U18">
-        <f>U17/U16</f>
+      <c r="V18">
+        <f>V17/V16</f>
         <v>0.25</v>
       </c>
-      <c r="V18" t="s">
+      <c r="W18" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C19">
+    <row r="19" spans="4:23" x14ac:dyDescent="0.4">
+      <c r="D19">
         <v>51</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>240</v>
       </c>
-      <c r="E19">
-        <f>1/(2*3.14*(C19*D19*10^(-21))^0.5)/1000000</f>
+      <c r="F19">
+        <f>1/(2*3.14*(D19*E19*10^(-21))^0.5)/1000000</f>
         <v>45.514486502788969</v>
       </c>
     </row>
-    <row r="20" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C20">
+    <row r="20" spans="4:23" x14ac:dyDescent="0.4">
+      <c r="D20">
         <v>510</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>2700</v>
       </c>
-      <c r="E20">
-        <f>1/(2*3.14*(C20*D20*10^(-21))^0.5)/1000000</f>
+      <c r="F20">
+        <f>1/(2*3.14*(D20*E20*10^(-21))^0.5)/1000000</f>
         <v>4.2911469397794235</v>
       </c>
     </row>
-    <row r="23" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="U23">
+    <row r="23" spans="4:23" x14ac:dyDescent="0.4">
+      <c r="V23">
         <v>3.3</v>
       </c>
     </row>
-    <row r="24" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="U24">
+    <row r="24" spans="4:23" x14ac:dyDescent="0.4">
+      <c r="V24">
         <v>1.27</v>
       </c>
     </row>
-    <row r="25" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="U25">
-        <f>U23-U24</f>
+    <row r="25" spans="4:23" x14ac:dyDescent="0.4">
+      <c r="V25">
+        <f>V23-V24</f>
         <v>2.0299999999999998</v>
       </c>
     </row>
-    <row r="26" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="U26">
-        <f>U25/2</f>
+    <row r="26" spans="4:23" x14ac:dyDescent="0.4">
+      <c r="V26">
+        <f>V25/2</f>
         <v>1.0149999999999999</v>
       </c>
     </row>
-    <row r="28" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="U28">
+    <row r="28" spans="4:23" x14ac:dyDescent="0.4">
+      <c r="V28">
         <v>1.27</v>
       </c>
     </row>
-    <row r="29" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="U29">
-        <f>U28/2</f>
+    <row r="29" spans="4:23" x14ac:dyDescent="0.4">
+      <c r="V29">
+        <f>V28/2</f>
         <v>0.63500000000000001</v>
       </c>
     </row>
+    <row r="48" spans="3:9" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C48" s="60" t="s">
+        <v>127</v>
+      </c>
+      <c r="D48" s="78" t="s">
+        <v>145</v>
+      </c>
+      <c r="E48" s="78" t="s">
+        <v>133</v>
+      </c>
+      <c r="F48" s="78" t="s">
+        <v>128</v>
+      </c>
+      <c r="G48" s="78" t="s">
+        <v>126</v>
+      </c>
+      <c r="H48" s="78" t="s">
+        <v>129</v>
+      </c>
+      <c r="I48" s="78" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C49" s="84">
+        <v>5</v>
+      </c>
+      <c r="D49" s="85">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="E49" s="85">
+        <v>1</v>
+      </c>
+      <c r="F49" s="85">
+        <v>1</v>
+      </c>
+      <c r="G49" s="85" t="s">
+        <v>130</v>
+      </c>
+      <c r="H49" s="85">
+        <v>1</v>
+      </c>
+      <c r="I49" s="85">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A51" s="119" t="s">
+        <v>158</v>
+      </c>
+      <c r="B51" s="120"/>
+      <c r="C51" s="120"/>
+      <c r="D51" s="120"/>
+      <c r="E51" s="120"/>
+      <c r="F51" s="120"/>
+      <c r="G51" s="120"/>
+      <c r="H51" s="20"/>
+      <c r="I51" s="20"/>
+      <c r="J51" s="20"/>
+      <c r="K51" s="20"/>
+      <c r="L51" s="95" t="s">
+        <v>124</v>
+      </c>
+      <c r="M51" s="95"/>
+      <c r="N51" s="95"/>
+      <c r="O51" s="95" t="s">
+        <v>125</v>
+      </c>
+      <c r="P51" s="95"/>
+      <c r="Q51" s="95"/>
+      <c r="R51" s="95" t="s">
+        <v>132</v>
+      </c>
+      <c r="S51" s="95"/>
+      <c r="T51" s="44"/>
+    </row>
+    <row r="52" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A52" s="73" t="s">
+        <v>131</v>
+      </c>
+      <c r="B52" s="78" t="s">
+        <v>154</v>
+      </c>
+      <c r="C52" s="78" t="s">
+        <v>155</v>
+      </c>
+      <c r="D52" s="78" t="s">
+        <v>147</v>
+      </c>
+      <c r="E52" s="78" t="s">
+        <v>150</v>
+      </c>
+      <c r="F52" s="78" t="s">
+        <v>148</v>
+      </c>
+      <c r="G52" s="78" t="s">
+        <v>151</v>
+      </c>
+      <c r="H52" s="78" t="s">
+        <v>149</v>
+      </c>
+      <c r="I52" s="78" t="s">
+        <v>152</v>
+      </c>
+      <c r="J52" s="78" t="s">
+        <v>113</v>
+      </c>
+      <c r="K52" s="78" t="s">
+        <v>144</v>
+      </c>
+      <c r="L52" s="78" t="s">
+        <v>137</v>
+      </c>
+      <c r="M52" s="78" t="s">
+        <v>138</v>
+      </c>
+      <c r="N52" s="79" t="s">
+        <v>139</v>
+      </c>
+      <c r="O52" s="78" t="s">
+        <v>137</v>
+      </c>
+      <c r="P52" s="78" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q52" s="79" t="s">
+        <v>139</v>
+      </c>
+      <c r="R52" s="78" t="s">
+        <v>146</v>
+      </c>
+      <c r="S52" s="78" t="s">
+        <v>2</v>
+      </c>
+      <c r="T52" s="80" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A53" s="121">
+        <v>0.64</v>
+      </c>
+      <c r="B53" s="20">
+        <v>300</v>
+      </c>
+      <c r="C53" s="20">
+        <v>220</v>
+      </c>
+      <c r="D53" s="20">
+        <v>1000</v>
+      </c>
+      <c r="E53" s="20">
+        <v>0</v>
+      </c>
+      <c r="F53" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="G53" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="H53" s="20">
+        <v>1000</v>
+      </c>
+      <c r="I53" s="20">
+        <v>0</v>
+      </c>
+      <c r="J53" s="122">
+        <v>0.3</v>
+      </c>
+      <c r="K53" s="122">
+        <f t="shared" ref="K53:K54" si="1">12*J53</f>
+        <v>3.5999999999999996</v>
+      </c>
+      <c r="L53" s="123">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="M53" s="123">
+        <v>0.27</v>
+      </c>
+      <c r="N53" s="123">
+        <f>L53/2*0.707</f>
+        <v>0.28845599999999999</v>
+      </c>
+      <c r="O53" s="123">
+        <v>17.2</v>
+      </c>
+      <c r="P53" s="123">
+        <v>6.07</v>
+      </c>
+      <c r="Q53" s="124">
+        <f>O53/2*0.707</f>
+        <v>6.0801999999999996</v>
+      </c>
+      <c r="R53" s="125">
+        <f t="shared" ref="R53:R54" si="2">O53/L53</f>
+        <v>21.078431372549019</v>
+      </c>
+      <c r="S53" s="125">
+        <f t="shared" ref="S53:S54" si="3">20*LOG(R53)</f>
+        <v>26.476765763073757</v>
+      </c>
+      <c r="T53" s="126">
+        <f t="shared" ref="T53:T54" si="4">P53*P53/50</f>
+        <v>0.73689800000000005</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A54" s="127">
+        <v>0.64</v>
+      </c>
+      <c r="B54" s="17">
+        <v>300</v>
+      </c>
+      <c r="C54" s="17">
+        <v>470</v>
+      </c>
+      <c r="D54" s="17">
+        <v>150</v>
+      </c>
+      <c r="E54" s="17">
+        <v>820</v>
+      </c>
+      <c r="F54" s="17">
+        <v>330</v>
+      </c>
+      <c r="G54" s="17">
+        <v>330</v>
+      </c>
+      <c r="H54" s="17">
+        <v>150</v>
+      </c>
+      <c r="I54" s="17">
+        <v>820</v>
+      </c>
+      <c r="J54" s="116">
+        <v>0.34</v>
+      </c>
+      <c r="K54" s="116">
+        <f t="shared" si="1"/>
+        <v>4.08</v>
+      </c>
+      <c r="L54" s="116">
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="M54" s="116">
+        <v>0.247</v>
+      </c>
+      <c r="N54" s="117">
+        <f>L54/2*0.707</f>
+        <v>0.26017599999999996</v>
+      </c>
+      <c r="O54" s="116">
+        <v>13.4</v>
+      </c>
+      <c r="P54" s="116">
+        <v>4.59</v>
+      </c>
+      <c r="Q54" s="118">
+        <f>O54/2*0.707</f>
+        <v>4.7368999999999994</v>
+      </c>
+      <c r="R54" s="77">
+        <f t="shared" si="2"/>
+        <v>18.206521739130437</v>
+      </c>
+      <c r="S54" s="77">
+        <f t="shared" si="3"/>
+        <v>25.204539680546176</v>
+      </c>
+      <c r="T54" s="128">
+        <f t="shared" si="4"/>
+        <v>0.42136199999999996</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A55" s="51">
+        <v>0.8</v>
+      </c>
+      <c r="B55" s="17"/>
+      <c r="C55" s="17"/>
+      <c r="D55" s="17"/>
+      <c r="E55" s="17"/>
+      <c r="F55" s="17"/>
+      <c r="G55" s="17"/>
+      <c r="H55" s="17"/>
+      <c r="I55" s="17"/>
+      <c r="J55" s="17">
+        <v>0.31</v>
+      </c>
+      <c r="K55" s="17"/>
+      <c r="L55" s="17">
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="M55" s="17">
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="N55" s="17"/>
+      <c r="O55" s="17">
+        <v>13.2</v>
+      </c>
+      <c r="P55" s="17">
+        <v>4.4400000000000004</v>
+      </c>
+      <c r="Q55" s="17"/>
+      <c r="R55" s="17"/>
+      <c r="S55" s="17"/>
+      <c r="T55" s="72"/>
+      <c r="U55" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A56" s="53">
+        <v>0.48</v>
+      </c>
+      <c r="B56" s="23"/>
+      <c r="C56" s="23"/>
+      <c r="D56" s="23"/>
+      <c r="E56" s="23"/>
+      <c r="F56" s="23"/>
+      <c r="G56" s="23"/>
+      <c r="H56" s="23"/>
+      <c r="I56" s="23"/>
+      <c r="J56" s="23">
+        <v>0.32</v>
+      </c>
+      <c r="K56" s="23"/>
+      <c r="L56" s="23">
+        <v>0.8</v>
+      </c>
+      <c r="M56" s="23">
+        <v>0.27100000000000002</v>
+      </c>
+      <c r="N56" s="23"/>
+      <c r="O56" s="23">
+        <v>13.2</v>
+      </c>
+      <c r="P56" s="23">
+        <v>4.57</v>
+      </c>
+      <c r="Q56" s="23"/>
+      <c r="R56" s="23"/>
+      <c r="S56" s="23"/>
+      <c r="T56" s="45"/>
+      <c r="U56" t="s">
+        <v>157</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="L51:N51"/>
+    <mergeCell ref="O51:Q51"/>
+    <mergeCell ref="R51:S51"/>
+    <mergeCell ref="A51:G51"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
@@ -3888,25 +5568,35 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2"/>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C78BB2F-A1AA-48EF-90B7-503CCC607E69}">
+  <dimension ref="B3:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T21" sqref="T21"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56.19921875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>104</v>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="C4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D4" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[PWR] Test results update
</commit_message>
<xml_diff>
--- a/Plasma RF Review data.xlsx
+++ b/Plasma RF Review data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE4A232-6420-4CF2-A493-B236479541F8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9264A7AF-CBF6-4438-B5A8-F523894DE173}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,15 +16,16 @@
     <sheet name="Check list" sheetId="5" r:id="rId6"/>
     <sheet name="Pre-Amp" sheetId="9" r:id="rId7"/>
     <sheet name="Path review" sheetId="7" r:id="rId8"/>
-    <sheet name="Debugging" sheetId="10" r:id="rId9"/>
-    <sheet name="FILTER" sheetId="8" r:id="rId10"/>
+    <sheet name="Sheet2" sheetId="11" r:id="rId9"/>
+    <sheet name="Debugging" sheetId="10" r:id="rId10"/>
+    <sheet name="FILTER" sheetId="8" r:id="rId11"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="203">
   <si>
     <t>Power</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -703,6 +704,178 @@
     <t>Icc[mA]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Vbias</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VR1 눈금</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>65도</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAIL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Load</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ω</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vrms</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vpp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vdc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Idc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>효율 100%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Iout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TX1_in</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gate_in</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Idc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>48VDC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OCP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TX1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1T:2T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1T:3T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Open</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.58V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vgs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vsd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vgd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정상</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>불량</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chip</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>board</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q1_in</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q1_out</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0,1,2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1T:2T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1T:3T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q2 12V bias Off 상태에서 측정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VR1 Voltage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>눈금</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VR2,3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q2 12V bias 및 48V Off 상태에서 측정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TX2가 75도 이상 상승하며, Idc가 증가함.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -712,7 +885,7 @@
     <numFmt numFmtId="176" formatCode="0.0"/>
     <numFmt numFmtId="177" formatCode="0.000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -767,8 +940,17 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -793,8 +975,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF99CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="37">
+  <borders count="40">
     <border>
       <left/>
       <right/>
@@ -1266,12 +1466,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="190">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -1463,6 +1702,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1541,6 +1789,122 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="6" fillId="5" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="6" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="176" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="6" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1548,6 +1912,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF99CC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1710,16 +2079,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>398780</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>213360</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>246380</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>297180</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1748,7 +2117,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5153660" y="4450080"/>
+          <a:off x="12819380" y="2263140"/>
           <a:ext cx="5415280" cy="4061460"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2314,15 +2683,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:P16"/>
+  <dimension ref="B3:P22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="2" width="5.09765625" customWidth="1"/>
+    <col min="7" max="7" width="12.8984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:16" ht="18" thickBot="1" x14ac:dyDescent="0.45">
@@ -2331,10 +2701,10 @@
       </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="C4" s="105" t="s">
+      <c r="C4" s="108" t="s">
         <v>115</v>
       </c>
-      <c r="D4" s="106"/>
+      <c r="D4" s="109"/>
       <c r="E4" s="20">
         <v>13.56</v>
       </c>
@@ -2347,10 +2717,10 @@
       </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="C5" s="103" t="s">
+      <c r="C5" s="106" t="s">
         <v>117</v>
       </c>
-      <c r="D5" s="104"/>
+      <c r="D5" s="107"/>
       <c r="E5" s="17">
         <v>50</v>
       </c>
@@ -2362,10 +2732,10 @@
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="C6" s="103" t="s">
+      <c r="C6" s="106" t="s">
         <v>119</v>
       </c>
-      <c r="D6" s="104"/>
+      <c r="D6" s="107"/>
       <c r="E6" s="17">
         <v>300</v>
       </c>
@@ -2376,148 +2746,235 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="2:16" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C7" s="101" t="s">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="C7" s="132"/>
+      <c r="D7" s="133" t="s">
+        <v>165</v>
+      </c>
+      <c r="E7" s="19">
+        <v>50</v>
+      </c>
+      <c r="F7" s="136" t="s">
+        <v>167</v>
+      </c>
+      <c r="G7" s="134"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="C8" s="132"/>
+      <c r="D8" s="137" t="s">
+        <v>166</v>
+      </c>
+      <c r="E8" s="135">
+        <f>(E6*E7)^0.5</f>
+        <v>122.47448713915891</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="G8" s="134"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="C9" s="132"/>
+      <c r="D9" s="138"/>
+      <c r="E9" s="135">
+        <f>E8*2/0.707</f>
+        <v>346.46248129889369</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="G9" s="134"/>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="C10" s="132"/>
+      <c r="D10" s="133" t="s">
+        <v>174</v>
+      </c>
+      <c r="E10" s="135">
+        <f>E6/E8</f>
+        <v>2.4494897427831779</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="G10" s="134"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="C11" s="132"/>
+      <c r="D11" s="133" t="s">
+        <v>171</v>
+      </c>
+      <c r="E11" s="135">
+        <v>48</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="G11" s="134"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="C12" s="132"/>
+      <c r="D12" s="133" t="s">
+        <v>172</v>
+      </c>
+      <c r="E12" s="135">
+        <f>E6/E11</f>
+        <v>6.25</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="G12" s="134" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C13" s="104" t="s">
         <v>121</v>
       </c>
-      <c r="D7" s="102"/>
-      <c r="E7" s="23">
+      <c r="D13" s="105"/>
+      <c r="E13" s="23">
         <v>30</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F13" s="23" t="s">
         <v>120</v>
       </c>
-      <c r="G7" s="45" t="s">
+      <c r="G13" s="45" t="s">
         <v>122</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L13" t="s">
         <v>0</v>
       </c>
-      <c r="M7">
+      <c r="M13">
         <v>1</v>
       </c>
-      <c r="N7">
+      <c r="N13">
         <v>100</v>
       </c>
-      <c r="O7">
+      <c r="O13">
         <v>300</v>
       </c>
-      <c r="P7" t="s">
+      <c r="P13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="M8">
-        <f>10*LOG(M7)</f>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="M14">
+        <f>10*LOG(M13)</f>
         <v>0</v>
       </c>
-      <c r="N8">
-        <f>10*LOG(N7)</f>
+      <c r="N14">
+        <f>10*LOG(N13)</f>
         <v>20</v>
       </c>
-      <c r="O8" s="1">
-        <f>10*LOG(O7)</f>
+      <c r="O14" s="1">
+        <f>10*LOG(O13)</f>
         <v>24.771212547196626</v>
       </c>
-      <c r="P8" t="s">
+      <c r="P14" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="M9">
-        <f>10*LOG(M7/0.001)</f>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="M15">
+        <f>10*LOG(M13/0.001)</f>
         <v>30</v>
       </c>
-      <c r="N9">
-        <f>10*LOG(N7/0.001)</f>
+      <c r="N15">
+        <f>10*LOG(N13/0.001)</f>
         <v>50</v>
       </c>
-      <c r="O9" s="1">
-        <f>10*LOG(O7/0.001)</f>
+      <c r="O15" s="1">
+        <f>10*LOG(O13/0.001)</f>
         <v>54.771212547196626</v>
       </c>
-      <c r="P9" t="s">
+      <c r="P15" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="L10" t="s">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="L16" t="s">
         <v>4</v>
       </c>
-      <c r="M10">
+      <c r="M16">
         <v>30</v>
       </c>
-      <c r="N10">
+      <c r="N16">
         <v>30</v>
       </c>
-      <c r="O10">
+      <c r="O16">
         <v>30</v>
       </c>
-      <c r="P10" t="s">
+      <c r="P16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="M11">
-        <f>M9-M10</f>
+    <row r="17" spans="6:16" x14ac:dyDescent="0.4">
+      <c r="F17" s="75">
+        <f>D17/2*0.707</f>
         <v>0</v>
       </c>
-      <c r="N11">
-        <f>N9-N10</f>
+      <c r="M17">
+        <f>M15-M16</f>
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <f>N15-N16</f>
         <v>20</v>
       </c>
-      <c r="O11" s="1">
-        <f>O9-O10</f>
+      <c r="O17" s="1">
+        <f>O15-O16</f>
         <v>24.771212547196626</v>
       </c>
-      <c r="P11" t="s">
+      <c r="P17" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="L14" t="s">
+    <row r="20" spans="6:16" x14ac:dyDescent="0.4">
+      <c r="L20" t="s">
         <v>6</v>
       </c>
-      <c r="N14" t="s">
+      <c r="N20" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="L15">
+    <row r="21" spans="6:16" x14ac:dyDescent="0.4">
+      <c r="L21">
         <v>12.56</v>
       </c>
-      <c r="M15" t="s">
+      <c r="M21" t="s">
         <v>69</v>
       </c>
-      <c r="N15" s="1">
-        <f>300/L15</f>
+      <c r="N21" s="1">
+        <f>300/L21</f>
         <v>23.885350318471335</v>
       </c>
-      <c r="O15" t="s">
+      <c r="O21" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="L16">
+    <row r="22" spans="6:16" x14ac:dyDescent="0.4">
+      <c r="L22">
         <v>13.56</v>
       </c>
-      <c r="M16" t="s">
+      <c r="M22" t="s">
         <v>69</v>
       </c>
-      <c r="N16" s="1">
-        <f>300/L16</f>
+      <c r="N22" s="1">
+        <f>300/L22</f>
         <v>22.123893805309734</v>
       </c>
-      <c r="O16" t="s">
+      <c r="O22" t="s">
         <v>71</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="C7:D7"/>
+  <mergeCells count="5">
+    <mergeCell ref="C13:D13"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C4:D4"/>
+    <mergeCell ref="D8:D9"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -2529,6 +2986,39 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C78BB2F-A1AA-48EF-90B7-503CCC607E69}">
+  <dimension ref="B3:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56.19921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="C4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B2"/>
   <sheetViews>
@@ -2594,7 +3084,7 @@
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B6" s="111" t="s">
+      <c r="B6" s="114" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="7" t="s">
@@ -2618,11 +3108,11 @@
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B7" s="112"/>
-      <c r="C7" s="107" t="s">
+      <c r="B7" s="115"/>
+      <c r="C7" s="110" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="109" t="s">
+      <c r="D7" s="112" t="s">
         <v>23</v>
       </c>
       <c r="E7" s="11">
@@ -2637,9 +3127,9 @@
       </c>
     </row>
     <row r="8" spans="2:11" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="113"/>
-      <c r="C8" s="108"/>
-      <c r="D8" s="110"/>
+      <c r="B8" s="116"/>
+      <c r="C8" s="111"/>
+      <c r="D8" s="113"/>
       <c r="E8" s="13">
         <v>12</v>
       </c>
@@ -2803,7 +3293,7 @@
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="C7" s="114" t="s">
+      <c r="C7" s="117" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="20" t="s">
@@ -2817,7 +3307,7 @@
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="C8" s="115"/>
+      <c r="C8" s="118"/>
       <c r="D8" s="17" t="s">
         <v>9</v>
       </c>
@@ -2829,7 +3319,7 @@
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="C9" s="115"/>
+      <c r="C9" s="118"/>
       <c r="D9" s="17" t="s">
         <v>10</v>
       </c>
@@ -2841,7 +3331,7 @@
       </c>
     </row>
     <row r="10" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C10" s="116"/>
+      <c r="C10" s="119"/>
       <c r="D10" s="19" t="s">
         <v>11</v>
       </c>
@@ -2854,7 +3344,7 @@
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="C11" s="114" t="s">
+      <c r="C11" s="117" t="s">
         <v>16</v>
       </c>
       <c r="D11" s="20" t="s">
@@ -2868,7 +3358,7 @@
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="C12" s="115"/>
+      <c r="C12" s="118"/>
       <c r="D12" s="17" t="s">
         <v>10</v>
       </c>
@@ -2880,7 +3370,7 @@
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="C13" s="115"/>
+      <c r="C13" s="118"/>
       <c r="D13" s="17" t="s">
         <v>13</v>
       </c>
@@ -2893,7 +3383,7 @@
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="C14" s="115"/>
+      <c r="C14" s="118"/>
       <c r="D14" s="17" t="s">
         <v>14</v>
       </c>
@@ -2905,7 +3395,7 @@
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="C15" s="115"/>
+      <c r="C15" s="118"/>
       <c r="D15" s="17" t="s">
         <v>15</v>
       </c>
@@ -2917,7 +3407,7 @@
       </c>
     </row>
     <row r="16" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C16" s="117"/>
+      <c r="C16" s="120"/>
       <c r="D16" s="23" t="s">
         <v>11</v>
       </c>
@@ -2960,7 +3450,7 @@
       </c>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.4">
-      <c r="C8" s="118" t="s">
+      <c r="C8" s="121" t="s">
         <v>56</v>
       </c>
       <c r="D8" s="15" t="s">
@@ -2983,7 +3473,7 @@
       </c>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.4">
-      <c r="C9" s="118"/>
+      <c r="C9" s="121"/>
       <c r="D9" s="15" t="s">
         <v>28</v>
       </c>
@@ -3001,7 +3491,7 @@
       </c>
     </row>
     <row r="10" spans="3:9" x14ac:dyDescent="0.4">
-      <c r="C10" s="118"/>
+      <c r="C10" s="121"/>
       <c r="D10" s="15" t="s">
         <v>29</v>
       </c>
@@ -3019,7 +3509,7 @@
       </c>
     </row>
     <row r="11" spans="3:9" x14ac:dyDescent="0.4">
-      <c r="C11" s="118"/>
+      <c r="C11" s="121"/>
       <c r="D11" s="15" t="s">
         <v>64</v>
       </c>
@@ -3040,7 +3530,7 @@
       </c>
     </row>
     <row r="12" spans="3:9" x14ac:dyDescent="0.4">
-      <c r="C12" s="118"/>
+      <c r="C12" s="121"/>
       <c r="D12" s="15" t="s">
         <v>30</v>
       </c>
@@ -3064,7 +3554,7 @@
       </c>
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.4">
-      <c r="C13" s="118"/>
+      <c r="C13" s="121"/>
       <c r="D13" s="15" t="s">
         <v>34</v>
       </c>
@@ -3088,7 +3578,7 @@
       </c>
     </row>
     <row r="14" spans="3:9" x14ac:dyDescent="0.4">
-      <c r="C14" s="118"/>
+      <c r="C14" s="121"/>
       <c r="D14" s="15" t="s">
         <v>35</v>
       </c>
@@ -3106,7 +3596,7 @@
       </c>
     </row>
     <row r="15" spans="3:9" x14ac:dyDescent="0.4">
-      <c r="C15" s="118"/>
+      <c r="C15" s="121"/>
       <c r="D15" s="15" t="s">
         <v>38</v>
       </c>
@@ -3239,19 +3729,19 @@
     </row>
     <row r="22" spans="4:14" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="23" spans="4:14" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="E23" s="122" t="s">
+      <c r="E23" s="125" t="s">
         <v>66</v>
       </c>
-      <c r="F23" s="123"/>
-      <c r="G23" s="123"/>
-      <c r="H23" s="120"/>
-      <c r="I23" s="121"/>
-      <c r="J23" s="119" t="s">
+      <c r="F23" s="126"/>
+      <c r="G23" s="126"/>
+      <c r="H23" s="123"/>
+      <c r="I23" s="124"/>
+      <c r="J23" s="122" t="s">
         <v>67</v>
       </c>
-      <c r="K23" s="120"/>
-      <c r="L23" s="120"/>
-      <c r="M23" s="121"/>
+      <c r="K23" s="123"/>
+      <c r="L23" s="123"/>
+      <c r="M23" s="124"/>
     </row>
     <row r="24" spans="4:14" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E24" s="37" t="s">
@@ -4240,10 +4730,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39AC99BC-2C16-460C-8540-F2312C53F795}">
-  <dimension ref="B3:S20"/>
+  <dimension ref="B3:S33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -4370,31 +4860,31 @@
       <c r="F10" s="71"/>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.4">
-      <c r="B11" s="124" t="s">
+      <c r="B11" s="127" t="s">
         <v>158</v>
       </c>
-      <c r="C11" s="125"/>
-      <c r="D11" s="125"/>
-      <c r="E11" s="125"/>
-      <c r="F11" s="125"/>
-      <c r="G11" s="125"/>
-      <c r="H11" s="126"/>
+      <c r="C11" s="128"/>
+      <c r="D11" s="128"/>
+      <c r="E11" s="128"/>
+      <c r="F11" s="128"/>
+      <c r="G11" s="128"/>
+      <c r="H11" s="129"/>
       <c r="I11" s="20"/>
       <c r="J11" s="20"/>
-      <c r="K11" s="106" t="s">
+      <c r="K11" s="109" t="s">
         <v>124</v>
       </c>
-      <c r="L11" s="106"/>
-      <c r="M11" s="106"/>
-      <c r="N11" s="106" t="s">
+      <c r="L11" s="109"/>
+      <c r="M11" s="109"/>
+      <c r="N11" s="109" t="s">
         <v>125</v>
       </c>
-      <c r="O11" s="106"/>
-      <c r="P11" s="106"/>
-      <c r="Q11" s="106" t="s">
+      <c r="O11" s="109"/>
+      <c r="P11" s="109"/>
+      <c r="Q11" s="109" t="s">
         <v>132</v>
       </c>
-      <c r="R11" s="106"/>
+      <c r="R11" s="109"/>
       <c r="S11" s="44"/>
     </row>
     <row r="12" spans="2:19" s="16" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
@@ -4866,6 +5356,7 @@
         <v>0.73689800000000005</v>
       </c>
     </row>
+    <row r="33" s="182" customFormat="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="K11:M11"/>
@@ -4884,8 +5375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A3:W56"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -5267,33 +5758,33 @@
     </row>
     <row r="50" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="51" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="A51" s="127" t="s">
+      <c r="A51" s="130" t="s">
         <v>158</v>
       </c>
-      <c r="B51" s="128"/>
-      <c r="C51" s="128"/>
-      <c r="D51" s="128"/>
-      <c r="E51" s="128"/>
-      <c r="F51" s="128"/>
-      <c r="G51" s="128"/>
+      <c r="B51" s="131"/>
+      <c r="C51" s="131"/>
+      <c r="D51" s="131"/>
+      <c r="E51" s="131"/>
+      <c r="F51" s="131"/>
+      <c r="G51" s="131"/>
       <c r="H51" s="20"/>
       <c r="I51" s="20"/>
       <c r="J51" s="20"/>
       <c r="K51" s="20"/>
-      <c r="L51" s="106" t="s">
+      <c r="L51" s="109" t="s">
         <v>124</v>
       </c>
-      <c r="M51" s="106"/>
-      <c r="N51" s="106"/>
-      <c r="O51" s="106" t="s">
+      <c r="M51" s="109"/>
+      <c r="N51" s="109"/>
+      <c r="O51" s="109" t="s">
         <v>125</v>
       </c>
-      <c r="P51" s="106"/>
-      <c r="Q51" s="106"/>
-      <c r="R51" s="106" t="s">
+      <c r="P51" s="109"/>
+      <c r="Q51" s="109"/>
+      <c r="R51" s="109" t="s">
         <v>132</v>
       </c>
-      <c r="S51" s="106"/>
+      <c r="S51" s="109"/>
       <c r="T51" s="44"/>
     </row>
     <row r="52" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.45">
@@ -5583,34 +6074,1598 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C78BB2F-A1AA-48EF-90B7-503CCC607E69}">
-  <dimension ref="B3:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76E8CB4C-2138-457F-AEBE-031CCCAABA8A}">
+  <dimension ref="B2:V47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="56.19921875" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:20" x14ac:dyDescent="0.4">
+      <c r="B2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="C4" t="s">
-        <v>135</v>
-      </c>
-      <c r="D4" t="s">
-        <v>136</v>
+        <v>110</v>
+      </c>
+      <c r="C3">
+        <v>2.5</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.4">
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.4">
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.4">
+      <c r="B6" t="s">
+        <v>160</v>
+      </c>
+      <c r="C6" s="1">
+        <f>12*C5/SUM(C3:C5)</f>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="D6" s="1">
+        <f>12*D5/SUM(D3:D5)</f>
+        <v>2.4</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.4">
+      <c r="B7" t="s">
+        <v>160</v>
+      </c>
+      <c r="C7">
+        <v>2.7120000000000002</v>
+      </c>
+      <c r="D7">
+        <v>2.33</v>
+      </c>
+      <c r="J7" s="143" t="s">
+        <v>188</v>
+      </c>
+      <c r="K7" s="143"/>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.4">
+      <c r="B8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8">
+        <v>0.18</v>
+      </c>
+      <c r="D8">
+        <v>0.04</v>
+      </c>
+      <c r="J8" t="s">
+        <v>190</v>
+      </c>
+      <c r="K8" t="s">
+        <v>191</v>
+      </c>
+      <c r="L8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.4">
+      <c r="B9" t="s">
+        <v>162</v>
+      </c>
+      <c r="C9">
+        <v>0.504</v>
+      </c>
+      <c r="D9">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="I9" t="s">
+        <v>185</v>
+      </c>
+      <c r="J9" t="s">
+        <v>183</v>
+      </c>
+      <c r="K9">
+        <v>0.46700000000000003</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.4">
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10">
+        <v>6.32</v>
+      </c>
+      <c r="D10">
+        <v>2.04</v>
+      </c>
+      <c r="I10" t="s">
+        <v>186</v>
+      </c>
+      <c r="J10" t="s">
+        <v>184</v>
+      </c>
+      <c r="K10">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="L10" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.4">
+      <c r="B11" t="s">
+        <v>163</v>
+      </c>
+      <c r="C11" t="s">
+        <v>164</v>
+      </c>
+      <c r="I11" t="s">
+        <v>187</v>
+      </c>
+      <c r="J11" t="s">
+        <v>183</v>
+      </c>
+      <c r="K11">
+        <v>0.82599999999999996</v>
+      </c>
+      <c r="L11">
+        <v>0.623</v>
+      </c>
+    </row>
+    <row r="13" spans="2:20" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.4">
+      <c r="B14" s="127"/>
+      <c r="C14" s="128"/>
+      <c r="D14" s="128"/>
+      <c r="E14" s="128"/>
+      <c r="F14" s="128"/>
+      <c r="G14" s="129"/>
+      <c r="H14" s="109" t="s">
+        <v>175</v>
+      </c>
+      <c r="I14" s="109"/>
+      <c r="J14" s="139"/>
+      <c r="K14" s="108" t="s">
+        <v>176</v>
+      </c>
+      <c r="L14" s="109"/>
+      <c r="M14" s="145"/>
+      <c r="N14" s="140" t="s">
+        <v>125</v>
+      </c>
+      <c r="O14" s="109"/>
+      <c r="P14" s="109"/>
+      <c r="Q14" s="109"/>
+      <c r="R14" s="103"/>
+      <c r="S14" s="109" t="s">
+        <v>178</v>
+      </c>
+      <c r="T14" s="145"/>
+    </row>
+    <row r="15" spans="2:20" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B15" s="101" t="s">
+        <v>127</v>
+      </c>
+      <c r="C15" s="102" t="s">
+        <v>126</v>
+      </c>
+      <c r="D15" s="102" t="s">
+        <v>131</v>
+      </c>
+      <c r="E15" s="102" t="s">
+        <v>180</v>
+      </c>
+      <c r="F15" s="102" t="s">
+        <v>113</v>
+      </c>
+      <c r="G15" s="102" t="s">
+        <v>144</v>
+      </c>
+      <c r="H15" s="102" t="s">
+        <v>137</v>
+      </c>
+      <c r="I15" s="102" t="s">
+        <v>138</v>
+      </c>
+      <c r="J15" s="148" t="s">
+        <v>139</v>
+      </c>
+      <c r="K15" s="101" t="s">
+        <v>137</v>
+      </c>
+      <c r="L15" s="102" t="s">
+        <v>138</v>
+      </c>
+      <c r="M15" s="153" t="s">
+        <v>139</v>
+      </c>
+      <c r="N15" s="149" t="s">
+        <v>137</v>
+      </c>
+      <c r="O15" s="102" t="s">
+        <v>138</v>
+      </c>
+      <c r="P15" s="79" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q15" s="79" t="s">
+        <v>21</v>
+      </c>
+      <c r="R15" s="79" t="s">
+        <v>132</v>
+      </c>
+      <c r="S15" s="146" t="s">
+        <v>177</v>
+      </c>
+      <c r="T15" s="147" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.4">
+      <c r="B16" s="48">
+        <v>6</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="D16" s="20">
+        <v>0.64</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="F16" s="20">
+        <v>0.01</v>
+      </c>
+      <c r="G16" s="160">
+        <f>12*F16</f>
+        <v>0.12</v>
+      </c>
+      <c r="H16" s="81">
+        <v>0.64</v>
+      </c>
+      <c r="I16" s="81">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="J16" s="163">
+        <f t="shared" ref="J16:J23" si="0">H16/2*0.707</f>
+        <v>0.22624</v>
+      </c>
+      <c r="K16" s="154">
+        <v>0.72</v>
+      </c>
+      <c r="L16" s="81">
+        <v>0.24</v>
+      </c>
+      <c r="M16" s="165">
+        <f t="shared" ref="M16:M23" si="1">K16/2*0.707</f>
+        <v>0.25451999999999997</v>
+      </c>
+      <c r="N16" s="150">
+        <v>28.4</v>
+      </c>
+      <c r="O16" s="82">
+        <v>9.94</v>
+      </c>
+      <c r="P16" s="174">
+        <f t="shared" ref="P16:P23" si="2">N16/2*0.707</f>
+        <v>10.039399999999999</v>
+      </c>
+      <c r="Q16" s="174">
+        <f>O16*O16/50</f>
+        <v>1.9760719999999998</v>
+      </c>
+      <c r="R16" s="175">
+        <f>20*LOG(N16/K16)</f>
+        <v>31.919716872315384</v>
+      </c>
+      <c r="S16" s="20">
+        <v>0.6</v>
+      </c>
+      <c r="T16" s="44">
+        <f>S16*48</f>
+        <v>28.799999999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="B17" s="51">
+        <v>5</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G17" s="161">
+        <f t="shared" ref="G17:G23" si="3">12*F17</f>
+        <v>0.84000000000000008</v>
+      </c>
+      <c r="H17" s="36">
+        <v>1.5</v>
+      </c>
+      <c r="I17" s="36">
+        <v>0.505</v>
+      </c>
+      <c r="J17" s="164">
+        <f t="shared" si="0"/>
+        <v>0.53025</v>
+      </c>
+      <c r="K17" s="38">
+        <v>1.74</v>
+      </c>
+      <c r="L17" s="36">
+        <v>0.58699999999999997</v>
+      </c>
+      <c r="M17" s="166">
+        <f t="shared" si="1"/>
+        <v>0.61508999999999991</v>
+      </c>
+      <c r="N17" s="151">
+        <v>95.2</v>
+      </c>
+      <c r="O17" s="76">
+        <v>33.6</v>
+      </c>
+      <c r="P17" s="175">
+        <f t="shared" si="2"/>
+        <v>33.653199999999998</v>
+      </c>
+      <c r="Q17" s="175">
+        <f t="shared" ref="Q17:Q23" si="4">O17*O17/50</f>
+        <v>22.5792</v>
+      </c>
+      <c r="R17" s="175">
+        <f>20*LOG(N17/K17)</f>
+        <v>34.761754002037492</v>
+      </c>
+      <c r="S17" s="17">
+        <v>2.7</v>
+      </c>
+      <c r="T17" s="72">
+        <f>S17*48</f>
+        <v>129.60000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="B18" s="179">
+        <v>4</v>
+      </c>
+      <c r="C18" s="180" t="s">
+        <v>140</v>
+      </c>
+      <c r="D18" s="180"/>
+      <c r="E18" s="180"/>
+      <c r="F18" s="180">
+        <v>0.45</v>
+      </c>
+      <c r="G18" s="180">
+        <f t="shared" si="3"/>
+        <v>5.4</v>
+      </c>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="164">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K18" s="155"/>
+      <c r="L18" s="36"/>
+      <c r="M18" s="166">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N18" s="152"/>
+      <c r="O18" s="76"/>
+      <c r="P18" s="175">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q18" s="175">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R18" s="175"/>
+      <c r="S18" s="17"/>
+      <c r="T18" s="72">
+        <f t="shared" ref="T18:T23" si="5">S18*48</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="B19" s="51">
+        <v>5</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="161">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H19" s="36">
+        <v>4.12</v>
+      </c>
+      <c r="I19" s="36">
+        <v>1.42</v>
+      </c>
+      <c r="J19" s="164">
+        <f t="shared" si="0"/>
+        <v>1.45642</v>
+      </c>
+      <c r="K19" s="155">
+        <v>4.88</v>
+      </c>
+      <c r="L19" s="36">
+        <v>1.7</v>
+      </c>
+      <c r="M19" s="166">
+        <f t="shared" si="1"/>
+        <v>1.7250799999999999</v>
+      </c>
+      <c r="N19" s="151">
+        <v>370</v>
+      </c>
+      <c r="O19" s="76">
+        <v>130</v>
+      </c>
+      <c r="P19" s="175">
+        <f t="shared" si="2"/>
+        <v>130.79499999999999</v>
+      </c>
+      <c r="Q19" s="175">
+        <f t="shared" si="4"/>
+        <v>338</v>
+      </c>
+      <c r="R19" s="175">
+        <f>20*LOG(N19/K19)</f>
+        <v>37.595638041285689</v>
+      </c>
+      <c r="S19" s="17"/>
+      <c r="T19" s="72">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="U19" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="B20" s="51">
+        <v>5</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="F20" s="17"/>
+      <c r="G20" s="161">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H20" s="36">
+        <v>1.76</v>
+      </c>
+      <c r="I20" s="36">
+        <v>0.57299999999999995</v>
+      </c>
+      <c r="J20" s="171">
+        <f t="shared" si="0"/>
+        <v>0.62215999999999994</v>
+      </c>
+      <c r="K20" s="155">
+        <v>3.24</v>
+      </c>
+      <c r="L20" s="36">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="M20" s="166">
+        <f t="shared" si="1"/>
+        <v>1.14534</v>
+      </c>
+      <c r="N20" s="151">
+        <v>88</v>
+      </c>
+      <c r="O20" s="76">
+        <v>29.6</v>
+      </c>
+      <c r="P20" s="175">
+        <f t="shared" si="2"/>
+        <v>31.107999999999997</v>
+      </c>
+      <c r="Q20" s="175">
+        <f t="shared" si="4"/>
+        <v>17.523200000000003</v>
+      </c>
+      <c r="R20" s="175">
+        <f>20*LOG(N20/K20)</f>
+        <v>28.678753238871128</v>
+      </c>
+      <c r="S20" s="17">
+        <v>1.7</v>
+      </c>
+      <c r="T20" s="72">
+        <f t="shared" si="5"/>
+        <v>81.599999999999994</v>
+      </c>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="B21" s="51"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="161">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H21" s="36"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="171">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K21" s="155"/>
+      <c r="L21" s="36"/>
+      <c r="M21" s="173">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N21" s="151"/>
+      <c r="O21" s="76"/>
+      <c r="P21" s="177">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q21" s="175">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R21" s="175" t="e">
+        <f t="shared" ref="R21:R23" si="6">20*LOG(N21/K21)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S21" s="17"/>
+      <c r="T21" s="72">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="B22" s="51"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="161">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H22" s="36"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="171">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K22" s="155"/>
+      <c r="L22" s="36"/>
+      <c r="M22" s="173">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N22" s="151"/>
+      <c r="O22" s="76"/>
+      <c r="P22" s="177">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q22" s="175">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R22" s="175" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S22" s="17"/>
+      <c r="T22" s="72">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:21" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B23" s="156"/>
+      <c r="C23" s="157"/>
+      <c r="D23" s="157"/>
+      <c r="E23" s="157"/>
+      <c r="F23" s="157"/>
+      <c r="G23" s="162">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H23" s="158"/>
+      <c r="I23" s="158"/>
+      <c r="J23" s="172">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K23" s="159"/>
+      <c r="L23" s="158"/>
+      <c r="M23" s="167">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N23" s="181"/>
+      <c r="O23" s="178"/>
+      <c r="P23" s="176">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q23" s="176">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R23" s="175" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S23" s="23"/>
+      <c r="T23" s="72">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:21" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B26" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="B27" s="127"/>
+      <c r="C27" s="128"/>
+      <c r="D27" s="128"/>
+      <c r="E27" s="128"/>
+      <c r="F27" s="128"/>
+      <c r="G27" s="128"/>
+      <c r="H27" s="129"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="109" t="s">
+        <v>192</v>
+      </c>
+      <c r="L27" s="109"/>
+      <c r="M27" s="109"/>
+      <c r="N27" s="109" t="s">
+        <v>193</v>
+      </c>
+      <c r="O27" s="109"/>
+      <c r="P27" s="109"/>
+      <c r="Q27" s="109" t="s">
+        <v>132</v>
+      </c>
+      <c r="R27" s="109"/>
+      <c r="S27" s="44"/>
+    </row>
+    <row r="28" spans="2:21" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B28" s="132" t="s">
+        <v>127</v>
+      </c>
+      <c r="C28" s="133" t="s">
+        <v>133</v>
+      </c>
+      <c r="D28" s="133" t="s">
+        <v>128</v>
+      </c>
+      <c r="E28" s="133" t="s">
+        <v>126</v>
+      </c>
+      <c r="F28" s="133" t="s">
+        <v>129</v>
+      </c>
+      <c r="G28" s="133" t="s">
+        <v>131</v>
+      </c>
+      <c r="H28" s="133" t="s">
+        <v>180</v>
+      </c>
+      <c r="I28" s="133" t="s">
+        <v>113</v>
+      </c>
+      <c r="J28" s="133" t="s">
+        <v>144</v>
+      </c>
+      <c r="K28" s="133" t="s">
+        <v>137</v>
+      </c>
+      <c r="L28" s="133" t="s">
+        <v>138</v>
+      </c>
+      <c r="M28" s="141" t="s">
+        <v>139</v>
+      </c>
+      <c r="N28" s="133" t="s">
+        <v>137</v>
+      </c>
+      <c r="O28" s="133" t="s">
+        <v>138</v>
+      </c>
+      <c r="P28" s="141" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q28" s="133" t="s">
+        <v>146</v>
+      </c>
+      <c r="R28" s="133" t="s">
+        <v>2</v>
+      </c>
+      <c r="S28" s="142" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="29" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="B29" s="48" t="s">
+        <v>194</v>
+      </c>
+      <c r="C29" s="20">
+        <v>1</v>
+      </c>
+      <c r="D29" s="20">
+        <v>1</v>
+      </c>
+      <c r="E29" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="F29" s="20">
+        <v>1</v>
+      </c>
+      <c r="G29" s="20">
+        <v>0.64</v>
+      </c>
+      <c r="H29" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="I29" s="20">
+        <v>0.19</v>
+      </c>
+      <c r="J29" s="20"/>
+      <c r="K29" s="81">
+        <v>0.45</v>
+      </c>
+      <c r="L29" s="81">
+        <v>0.15</v>
+      </c>
+      <c r="M29" s="74">
+        <f>K29/2*0.707</f>
+        <v>0.15907499999999999</v>
+      </c>
+      <c r="N29" s="82">
+        <v>0</v>
+      </c>
+      <c r="O29" s="81">
+        <v>0</v>
+      </c>
+      <c r="P29" s="74">
+        <f>N29/2*0.707</f>
+        <v>0</v>
+      </c>
+      <c r="Q29" s="82">
+        <f>N29/K29</f>
+        <v>0</v>
+      </c>
+      <c r="R29" s="82" t="e">
+        <f>20*LOG(Q29)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="S29" s="44"/>
+    </row>
+    <row r="30" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="B30" s="51">
+        <v>3</v>
+      </c>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="17"/>
+      <c r="K30" s="36">
+        <v>0.45</v>
+      </c>
+      <c r="L30" s="36">
+        <v>0.15</v>
+      </c>
+      <c r="M30" s="75">
+        <f>K30/2*0.707</f>
+        <v>0.15907499999999999</v>
+      </c>
+      <c r="N30" s="76">
+        <v>0.17</v>
+      </c>
+      <c r="O30" s="36">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="P30" s="75">
+        <f>N30/2*0.707</f>
+        <v>6.0095000000000003E-2</v>
+      </c>
+      <c r="Q30" s="76">
+        <f>N30/K30</f>
+        <v>0.37777777777777777</v>
+      </c>
+      <c r="R30" s="76">
+        <f>20*LOG(Q30)</f>
+        <v>-8.4552718479413951</v>
+      </c>
+      <c r="S30" s="83">
+        <f>O30*O30/50</f>
+        <v>6.4980000000000005E-5</v>
+      </c>
+    </row>
+    <row r="31" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="B31" s="51">
+        <v>4</v>
+      </c>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17">
+        <v>0.22</v>
+      </c>
+      <c r="J31" s="17"/>
+      <c r="K31" s="36">
+        <v>0.45</v>
+      </c>
+      <c r="L31" s="36">
+        <v>0.15</v>
+      </c>
+      <c r="M31" s="75">
+        <f>K31/2*0.707</f>
+        <v>0.15907499999999999</v>
+      </c>
+      <c r="N31" s="36">
+        <v>1.03</v>
+      </c>
+      <c r="O31" s="36">
+        <v>0.36599999999999999</v>
+      </c>
+      <c r="P31" s="75">
+        <f>N31/2*0.707</f>
+        <v>0.36410500000000001</v>
+      </c>
+      <c r="Q31" s="76">
+        <f>N31/K31</f>
+        <v>2.2888888888888888</v>
+      </c>
+      <c r="R31" s="76">
+        <f>20*LOG(Q31)</f>
+        <v>7.1924942185965701</v>
+      </c>
+      <c r="S31" s="83">
+        <f>O31*O31/50</f>
+        <v>2.6791199999999997E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="B32" s="51">
+        <v>5</v>
+      </c>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="17">
+        <v>0.3</v>
+      </c>
+      <c r="J32" s="17"/>
+      <c r="K32" s="36">
+        <v>0.45</v>
+      </c>
+      <c r="L32" s="36">
+        <v>0.15</v>
+      </c>
+      <c r="M32" s="75">
+        <f>K32/2*0.707</f>
+        <v>0.15907499999999999</v>
+      </c>
+      <c r="N32" s="36">
+        <v>3.24</v>
+      </c>
+      <c r="O32" s="36">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="P32" s="75">
+        <f>N32/2*0.707</f>
+        <v>1.14534</v>
+      </c>
+      <c r="Q32" s="76">
+        <f>N32/K32</f>
+        <v>7.2</v>
+      </c>
+      <c r="R32" s="76">
+        <f>20*LOG(Q32)</f>
+        <v>17.146649928625372</v>
+      </c>
+      <c r="S32" s="83">
+        <f>O32*O32/50</f>
+        <v>2.5537999999999995E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:22" x14ac:dyDescent="0.4">
+      <c r="B33" s="51">
+        <v>5</v>
+      </c>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="17">
+        <v>0.27</v>
+      </c>
+      <c r="J33" s="17"/>
+      <c r="K33" s="36">
+        <v>0.3</v>
+      </c>
+      <c r="L33" s="36">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="M33" s="36">
+        <f>K33/2*0.707</f>
+        <v>0.10604999999999999</v>
+      </c>
+      <c r="N33" s="36">
+        <v>1.38</v>
+      </c>
+      <c r="O33" s="36">
+        <v>0.48</v>
+      </c>
+      <c r="P33" s="75">
+        <f>N33/2*0.707</f>
+        <v>0.48782999999999993</v>
+      </c>
+      <c r="Q33" s="76">
+        <f>N33/K33</f>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="R33" s="76">
+        <f>20*LOG(Q33)</f>
+        <v>13.255156633631483</v>
+      </c>
+      <c r="S33" s="83">
+        <f>O33*O33/50</f>
+        <v>4.6080000000000001E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="2:22" x14ac:dyDescent="0.4">
+      <c r="B34" s="51">
+        <v>5</v>
+      </c>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17">
+        <v>1.2</v>
+      </c>
+      <c r="H34" s="17"/>
+      <c r="I34" s="17">
+        <v>0.26</v>
+      </c>
+      <c r="J34" s="17"/>
+      <c r="K34" s="36">
+        <v>0.3</v>
+      </c>
+      <c r="L34" s="36"/>
+      <c r="M34" s="36">
+        <f>K34/2*0.707</f>
+        <v>0.10604999999999999</v>
+      </c>
+      <c r="N34" s="36">
+        <v>1.38</v>
+      </c>
+      <c r="O34" s="36"/>
+      <c r="P34" s="36">
+        <f>N34/2*0.707</f>
+        <v>0.48782999999999993</v>
+      </c>
+      <c r="Q34" s="76">
+        <f>N34/K34</f>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="R34" s="76">
+        <f>20*LOG(Q34)</f>
+        <v>13.255156633631483</v>
+      </c>
+      <c r="S34" s="83">
+        <f>O34*O34/50</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:22" x14ac:dyDescent="0.4">
+      <c r="B35" s="51">
+        <v>5</v>
+      </c>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17">
+        <v>1.2</v>
+      </c>
+      <c r="H35" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="I35" s="17">
+        <v>0.27</v>
+      </c>
+      <c r="J35" s="17"/>
+      <c r="K35" s="36">
+        <v>0.3</v>
+      </c>
+      <c r="L35" s="36"/>
+      <c r="M35" s="36">
+        <f>K35/2*0.707</f>
+        <v>0.10604999999999999</v>
+      </c>
+      <c r="N35" s="36">
+        <v>0.78</v>
+      </c>
+      <c r="O35" s="36">
+        <v>0.26</v>
+      </c>
+      <c r="P35" s="36">
+        <f>N35/2*0.707</f>
+        <v>0.27572999999999998</v>
+      </c>
+      <c r="Q35" s="77">
+        <f>N35/K35</f>
+        <v>2.6</v>
+      </c>
+      <c r="R35" s="76">
+        <f>20*LOG(Q35)</f>
+        <v>8.2994669594163604</v>
+      </c>
+      <c r="S35" s="83">
+        <f>O35*O35/50</f>
+        <v>1.3520000000000001E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="2:22" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B36" s="84">
+        <v>4</v>
+      </c>
+      <c r="C36" s="85">
+        <v>1</v>
+      </c>
+      <c r="D36" s="85">
+        <v>1</v>
+      </c>
+      <c r="E36" s="85" t="s">
+        <v>140</v>
+      </c>
+      <c r="F36" s="85">
+        <v>1</v>
+      </c>
+      <c r="G36" s="85">
+        <v>1.2</v>
+      </c>
+      <c r="H36" s="85" t="s">
+        <v>196</v>
+      </c>
+      <c r="I36" s="85">
+        <v>0.22</v>
+      </c>
+      <c r="J36" s="85"/>
+      <c r="K36" s="86">
+        <v>0.36399999999999999</v>
+      </c>
+      <c r="L36" s="86">
+        <v>0.123</v>
+      </c>
+      <c r="M36" s="86">
+        <f>K36/2*0.707</f>
+        <v>0.12867399999999998</v>
+      </c>
+      <c r="N36" s="86">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="O36" s="86">
+        <v>0.154</v>
+      </c>
+      <c r="P36" s="87">
+        <f>N36/2*0.707</f>
+        <v>0.17250799999999999</v>
+      </c>
+      <c r="Q36" s="88">
+        <f>N36/K36</f>
+        <v>1.3406593406593406</v>
+      </c>
+      <c r="R36" s="88">
+        <f>20*LOG(Q36)</f>
+        <v>2.5463687670730915</v>
+      </c>
+      <c r="S36" s="89">
+        <f>O36*O36/50</f>
+        <v>4.7432000000000003E-4</v>
+      </c>
+    </row>
+    <row r="37" spans="2:22" x14ac:dyDescent="0.4">
+      <c r="B37" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="38" spans="2:22" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B38">
+        <v>2.3719999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="2:22" x14ac:dyDescent="0.4">
+      <c r="B39" s="108" t="s">
+        <v>110</v>
+      </c>
+      <c r="C39" s="109"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="109" t="s">
+        <v>200</v>
+      </c>
+      <c r="I39" s="109"/>
+      <c r="J39" s="109" t="s">
+        <v>175</v>
+      </c>
+      <c r="K39" s="109"/>
+      <c r="L39" s="109"/>
+      <c r="M39" s="109" t="s">
+        <v>176</v>
+      </c>
+      <c r="N39" s="109"/>
+      <c r="O39" s="109"/>
+      <c r="P39" s="109" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q39" s="109"/>
+      <c r="R39" s="109"/>
+      <c r="S39" s="109"/>
+      <c r="T39" s="103"/>
+      <c r="U39" s="109" t="s">
+        <v>178</v>
+      </c>
+      <c r="V39" s="145"/>
+    </row>
+    <row r="40" spans="2:22" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B40" s="132" t="s">
+        <v>199</v>
+      </c>
+      <c r="C40" s="133" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" s="133" t="s">
+        <v>126</v>
+      </c>
+      <c r="E40" s="133" t="s">
+        <v>131</v>
+      </c>
+      <c r="F40" s="133" t="s">
+        <v>180</v>
+      </c>
+      <c r="G40" s="133" t="s">
+        <v>113</v>
+      </c>
+      <c r="H40" s="133" t="s">
+        <v>199</v>
+      </c>
+      <c r="I40" s="133" t="s">
+        <v>7</v>
+      </c>
+      <c r="J40" s="133" t="s">
+        <v>137</v>
+      </c>
+      <c r="K40" s="133" t="s">
+        <v>138</v>
+      </c>
+      <c r="L40" s="141" t="s">
+        <v>139</v>
+      </c>
+      <c r="M40" s="133" t="s">
+        <v>137</v>
+      </c>
+      <c r="N40" s="133" t="s">
+        <v>138</v>
+      </c>
+      <c r="O40" s="141" t="s">
+        <v>139</v>
+      </c>
+      <c r="P40" s="133" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q40" s="133" t="s">
+        <v>138</v>
+      </c>
+      <c r="R40" s="141" t="s">
+        <v>139</v>
+      </c>
+      <c r="S40" s="141" t="s">
+        <v>21</v>
+      </c>
+      <c r="T40" s="141" t="s">
+        <v>132</v>
+      </c>
+      <c r="U40" s="144" t="s">
+        <v>177</v>
+      </c>
+      <c r="V40" s="188" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="2:22" x14ac:dyDescent="0.4">
+      <c r="B41" s="93">
+        <v>4.5</v>
+      </c>
+      <c r="C41" s="187">
+        <v>2.3719999999999999</v>
+      </c>
+      <c r="D41" s="187" t="s">
+        <v>140</v>
+      </c>
+      <c r="E41" s="187">
+        <v>1.2</v>
+      </c>
+      <c r="F41" s="187" t="s">
+        <v>196</v>
+      </c>
+      <c r="G41" s="20">
+        <v>0.23</v>
+      </c>
+      <c r="H41" s="187">
+        <v>5</v>
+      </c>
+      <c r="I41" s="187">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="J41" s="81">
+        <v>0.48</v>
+      </c>
+      <c r="K41" s="81">
+        <v>0.17</v>
+      </c>
+      <c r="L41" s="168">
+        <f t="shared" ref="L41:L45" si="7">J41/2*0.707</f>
+        <v>0.16968</v>
+      </c>
+      <c r="M41" s="82">
+        <v>0.88</v>
+      </c>
+      <c r="N41" s="81">
+        <v>0.3</v>
+      </c>
+      <c r="O41" s="168">
+        <f t="shared" ref="O41:O45" si="8">M41/2*0.707</f>
+        <v>0.31107999999999997</v>
+      </c>
+      <c r="P41" s="183" t="s">
+        <v>201</v>
+      </c>
+      <c r="Q41" s="183"/>
+      <c r="R41" s="184"/>
+      <c r="S41" s="184"/>
+      <c r="T41" s="184"/>
+      <c r="U41" s="185"/>
+      <c r="V41" s="186"/>
+    </row>
+    <row r="42" spans="2:22" x14ac:dyDescent="0.4">
+      <c r="B42" s="51"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="17">
+        <v>0.36</v>
+      </c>
+      <c r="H42" s="90">
+        <v>5</v>
+      </c>
+      <c r="I42" s="90">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="J42" s="36">
+        <v>2.92</v>
+      </c>
+      <c r="K42" s="36">
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="L42" s="169">
+        <f t="shared" si="7"/>
+        <v>1.0322199999999999</v>
+      </c>
+      <c r="M42" s="76">
+        <v>6.32</v>
+      </c>
+      <c r="N42" s="36">
+        <v>1.85</v>
+      </c>
+      <c r="O42" s="169">
+        <f t="shared" si="8"/>
+        <v>2.2341199999999999</v>
+      </c>
+      <c r="P42" s="76">
+        <v>426</v>
+      </c>
+      <c r="Q42" s="76">
+        <v>142</v>
+      </c>
+      <c r="R42" s="175">
+        <f>P42/2*0.707</f>
+        <v>150.59099999999998</v>
+      </c>
+      <c r="S42" s="175">
+        <f t="shared" ref="S42" si="9">Q42*Q42/50</f>
+        <v>403.28</v>
+      </c>
+      <c r="T42" s="175">
+        <f>20*LOG(P42/M42)</f>
+        <v>36.573850416406678</v>
+      </c>
+      <c r="U42" s="17">
+        <v>4</v>
+      </c>
+      <c r="V42" s="72">
+        <f>U42*48</f>
+        <v>192</v>
+      </c>
+    </row>
+    <row r="43" spans="2:22" x14ac:dyDescent="0.4">
+      <c r="B43" s="51"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="17">
+        <v>0.36</v>
+      </c>
+      <c r="H43" s="17">
+        <v>4</v>
+      </c>
+      <c r="I43" s="17">
+        <v>2.2949999999999999</v>
+      </c>
+      <c r="J43" s="17"/>
+      <c r="K43" s="17"/>
+      <c r="L43" s="17"/>
+      <c r="M43" s="17"/>
+      <c r="N43" s="17"/>
+      <c r="O43" s="17"/>
+      <c r="P43" s="17"/>
+      <c r="Q43" s="17"/>
+      <c r="R43" s="17"/>
+      <c r="S43" s="17"/>
+      <c r="T43" s="17"/>
+      <c r="U43" s="17">
+        <v>3.9</v>
+      </c>
+      <c r="V43" s="72">
+        <f>U43*48</f>
+        <v>187.2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:22" x14ac:dyDescent="0.4">
+      <c r="B44" s="51">
+        <v>4</v>
+      </c>
+      <c r="C44" s="17">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D44" s="17"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="17">
+        <v>0.36</v>
+      </c>
+      <c r="H44" s="17">
+        <v>5</v>
+      </c>
+      <c r="I44" s="17"/>
+      <c r="J44" s="17">
+        <v>3.26</v>
+      </c>
+      <c r="K44" s="17">
+        <v>1.07</v>
+      </c>
+      <c r="L44" s="169">
+        <f t="shared" si="7"/>
+        <v>1.1524099999999999</v>
+      </c>
+      <c r="M44" s="17">
+        <v>6.88</v>
+      </c>
+      <c r="N44" s="17">
+        <v>2.21</v>
+      </c>
+      <c r="O44" s="169">
+        <f t="shared" si="8"/>
+        <v>2.43208</v>
+      </c>
+      <c r="P44" s="17">
+        <v>416</v>
+      </c>
+      <c r="Q44" s="17">
+        <v>143</v>
+      </c>
+      <c r="R44" s="175">
+        <f>P44/2*0.707</f>
+        <v>147.05599999999998</v>
+      </c>
+      <c r="S44" s="175">
+        <f t="shared" ref="S44" si="10">Q44*Q44/50</f>
+        <v>408.98</v>
+      </c>
+      <c r="T44" s="175">
+        <f>20*LOG(P44/M44)</f>
+        <v>35.630097847824629</v>
+      </c>
+      <c r="U44" s="17"/>
+      <c r="V44" s="72"/>
+    </row>
+    <row r="45" spans="2:22" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B45" s="53">
+        <v>4</v>
+      </c>
+      <c r="C45" s="23">
+        <v>2.3220000000000001</v>
+      </c>
+      <c r="D45" s="23"/>
+      <c r="E45" s="23"/>
+      <c r="F45" s="23"/>
+      <c r="G45" s="157">
+        <v>0.36</v>
+      </c>
+      <c r="H45" s="157">
+        <v>4</v>
+      </c>
+      <c r="I45" s="157">
+        <v>2.27</v>
+      </c>
+      <c r="J45" s="157">
+        <v>3.38</v>
+      </c>
+      <c r="K45" s="157">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="L45" s="170">
+        <f t="shared" si="7"/>
+        <v>1.1948299999999998</v>
+      </c>
+      <c r="M45" s="23">
+        <v>6.92</v>
+      </c>
+      <c r="N45" s="23">
+        <v>2.21</v>
+      </c>
+      <c r="O45" s="170">
+        <f t="shared" si="8"/>
+        <v>2.4462199999999998</v>
+      </c>
+      <c r="P45" s="23">
+        <v>374</v>
+      </c>
+      <c r="Q45" s="23">
+        <v>129</v>
+      </c>
+      <c r="R45" s="176">
+        <f>P45/2*0.707</f>
+        <v>132.209</v>
+      </c>
+      <c r="S45" s="176">
+        <f t="shared" ref="S45" si="11">Q45*Q45/50</f>
+        <v>332.82</v>
+      </c>
+      <c r="T45" s="176">
+        <f>20*LOG(P45/M45)</f>
+        <v>34.655310154874442</v>
+      </c>
+      <c r="U45" s="23">
+        <v>3.9</v>
+      </c>
+      <c r="V45" s="45">
+        <f>U45*48</f>
+        <v>187.2</v>
+      </c>
+    </row>
+    <row r="46" spans="2:22" x14ac:dyDescent="0.4">
+      <c r="B46" s="189" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="47" spans="2:22" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="P47" s="23">
+        <v>360</v>
+      </c>
+      <c r="Q47" s="23">
+        <v>117</v>
+      </c>
+      <c r="R47" s="175">
+        <f>P47/2*0.707</f>
+        <v>127.25999999999999</v>
+      </c>
+      <c r="S47" s="175">
+        <f t="shared" ref="S47" si="12">Q47*Q47/50</f>
+        <v>273.77999999999997</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="J39:L39"/>
+    <mergeCell ref="M39:O39"/>
+    <mergeCell ref="P39:S39"/>
+    <mergeCell ref="U39:V39"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="S14:T14"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="B27:H27"/>
+    <mergeCell ref="K27:M27"/>
+    <mergeCell ref="N27:P27"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="N14:Q14"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>